<commit_message>
Rename ConsoleCatchall => Reconciliate
</commit_message>
<xml_diff>
--- a/spreadsheet-samples/Test-Spreadsheet.xlsx
+++ b/spreadsheet-samples/Test-Spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\Reconciliate\spreadsheet-samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B556991-1EAF-42F4-8410-D77840578124}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{311460D6-0676-40DF-92E8-FAC272E2B635}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25200" yWindow="2850" windowWidth="18000" windowHeight="9360" firstSheet="5" activeTab="9" xr2:uid="{E73E5FC3-A692-4EF9-93A1-0012994854D9}"/>
   </bookViews>
@@ -336,10 +336,10 @@
     <t>ABC</t>
   </si>
   <si>
-    <t>Description007zzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzz</t>
-  </si>
-  <si>
-    <t>some test textzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzz</t>
+    <t>Description007zzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzz</t>
+  </si>
+  <si>
+    <t>some test textzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzz</t>
   </si>
 </sst>
 </file>
@@ -1067,7 +1067,7 @@
       </c>
       <c r="B1" s="24">
         <f>SUM(B2:B295)</f>
-        <v>9632.1949999999997</v>
+        <v>9634.5950000000012</v>
       </c>
       <c r="C1" s="25"/>
       <c r="D1" s="25" t="s">
@@ -1191,7 +1191,7 @@
         <v>36</v>
       </c>
       <c r="B9" s="27">
-        <v>1322.96</v>
+        <v>1324.16</v>
       </c>
       <c r="C9" s="28"/>
       <c r="D9" s="30" t="s">
@@ -1223,7 +1223,7 @@
         <v>37</v>
       </c>
       <c r="B11" s="27">
-        <v>419.62</v>
+        <v>420.82</v>
       </c>
       <c r="C11" s="28"/>
       <c r="D11" s="30" t="s">
@@ -2065,10 +2065,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>43217</v>
+        <v>43218</v>
       </c>
       <c r="B10" s="5">
-        <v>65.94</v>
+        <v>67.14</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
@@ -2389,7 +2389,7 @@
         <v>43405</v>
       </c>
       <c r="C9" s="19">
-        <v>81.819999999999993</v>
+        <v>83.02</v>
       </c>
       <c r="D9" s="19"/>
       <c r="E9" s="21" t="s">

</xml_diff>

<commit_message>
Slow test refactor: Ignore Excel tests > 100ms
</commit_message>
<xml_diff>
--- a/spreadsheet-samples/Test-Spreadsheet.xlsx
+++ b/spreadsheet-samples/Test-Spreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\Reconciliate\spreadsheet-samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{311460D6-0676-40DF-92E8-FAC272E2B635}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E35855F-1F2A-44F4-B5A6-136AF0F05C21}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25200" yWindow="2850" windowWidth="18000" windowHeight="9360" firstSheet="5" activeTab="9" xr2:uid="{E73E5FC3-A692-4EF9-93A1-0012994854D9}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="18000" windowHeight="9360" firstSheet="5" activeTab="9" xr2:uid="{E73E5FC3-A692-4EF9-93A1-0012994854D9}"/>
   </bookViews>
   <sheets>
     <sheet name="Bank" sheetId="7" r:id="rId1"/>
@@ -336,10 +336,10 @@
     <t>ABC</t>
   </si>
   <si>
-    <t>Description007zzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzz</t>
-  </si>
-  <si>
-    <t>some test textzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzz</t>
+    <t>Description007zzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzz</t>
+  </si>
+  <si>
+    <t>some test textzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzz</t>
   </si>
 </sst>
 </file>
@@ -1067,7 +1067,7 @@
       </c>
       <c r="B1" s="24">
         <f>SUM(B2:B295)</f>
-        <v>9634.5950000000012</v>
+        <v>9638.1949999999997</v>
       </c>
       <c r="C1" s="25"/>
       <c r="D1" s="25" t="s">
@@ -1191,7 +1191,7 @@
         <v>36</v>
       </c>
       <c r="B9" s="27">
-        <v>1324.16</v>
+        <v>1326.56</v>
       </c>
       <c r="C9" s="28"/>
       <c r="D9" s="30" t="s">
@@ -1223,7 +1223,7 @@
         <v>37</v>
       </c>
       <c r="B11" s="27">
-        <v>420.82</v>
+        <v>422.02</v>
       </c>
       <c r="C11" s="28"/>
       <c r="D11" s="30" t="s">
@@ -2065,10 +2065,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>43218</v>
+        <v>43220</v>
       </c>
       <c r="B10" s="5">
-        <v>67.14</v>
+        <v>69.540000000000006</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
@@ -2389,7 +2389,7 @@
         <v>43405</v>
       </c>
       <c r="C9" s="19">
-        <v>83.02</v>
+        <v>84.22</v>
       </c>
       <c r="D9" s="19"/>
       <c r="E9" s="21" t="s">

</xml_diff>

<commit_message>
Add notes about the slow test refactor.
</commit_message>
<xml_diff>
--- a/spreadsheet-samples/Test-Spreadsheet.xlsx
+++ b/spreadsheet-samples/Test-Spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\Reconciliate\spreadsheet-samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E35855F-1F2A-44F4-B5A6-136AF0F05C21}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E8AF3B5-826C-4831-8915-263D150F0FB2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="780" windowWidth="18000" windowHeight="9360" firstSheet="5" activeTab="9" xr2:uid="{E73E5FC3-A692-4EF9-93A1-0012994854D9}"/>
   </bookViews>
@@ -339,7 +339,7 @@
     <t>Description007zzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzz</t>
   </si>
   <si>
-    <t>some test textzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzz</t>
+    <t>some test textzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzz</t>
   </si>
 </sst>
 </file>
@@ -1067,7 +1067,7 @@
       </c>
       <c r="B1" s="24">
         <f>SUM(B2:B295)</f>
-        <v>9638.1949999999997</v>
+        <v>9639.3950000000004</v>
       </c>
       <c r="C1" s="25"/>
       <c r="D1" s="25" t="s">
@@ -1191,7 +1191,7 @@
         <v>36</v>
       </c>
       <c r="B9" s="27">
-        <v>1326.56</v>
+        <v>1327.76</v>
       </c>
       <c r="C9" s="28"/>
       <c r="D9" s="30" t="s">
@@ -2065,10 +2065,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>43220</v>
+        <v>43221</v>
       </c>
       <c r="B10" s="5">
-        <v>69.540000000000006</v>
+        <v>70.739999999999995</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Stop ignoring Excel record tests.
</commit_message>
<xml_diff>
--- a/spreadsheet-samples/Test-Spreadsheet.xlsx
+++ b/spreadsheet-samples/Test-Spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\Reconciliate\spreadsheet-samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E8AF3B5-826C-4831-8915-263D150F0FB2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29FC86E9-12E8-454F-88A3-E5CE4FEBD105}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="780" windowWidth="18000" windowHeight="9360" firstSheet="5" activeTab="9" xr2:uid="{E73E5FC3-A692-4EF9-93A1-0012994854D9}"/>
   </bookViews>
@@ -339,7 +339,7 @@
     <t>Description007zzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzz</t>
   </si>
   <si>
-    <t>some test textzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzz</t>
+    <t>some test textzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzz</t>
   </si>
 </sst>
 </file>
@@ -1067,7 +1067,7 @@
       </c>
       <c r="B1" s="24">
         <f>SUM(B2:B295)</f>
-        <v>9639.3950000000004</v>
+        <v>9640.5950000000012</v>
       </c>
       <c r="C1" s="25"/>
       <c r="D1" s="25" t="s">
@@ -1191,7 +1191,7 @@
         <v>36</v>
       </c>
       <c r="B9" s="27">
-        <v>1327.76</v>
+        <v>1328.96</v>
       </c>
       <c r="C9" s="28"/>
       <c r="D9" s="30" t="s">
@@ -2065,10 +2065,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>43221</v>
+        <v>43222</v>
       </c>
       <c r="B10" s="5">
-        <v>70.739999999999995</v>
+        <v>71.94</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
More notes on slow tests
</commit_message>
<xml_diff>
--- a/spreadsheet-samples/Test-Spreadsheet.xlsx
+++ b/spreadsheet-samples/Test-Spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\Reconciliate\spreadsheet-samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29FC86E9-12E8-454F-88A3-E5CE4FEBD105}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9144FB6F-53BB-40A5-A402-CAB641F3E825}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="780" windowWidth="18000" windowHeight="9360" firstSheet="5" activeTab="9" xr2:uid="{E73E5FC3-A692-4EF9-93A1-0012994854D9}"/>
   </bookViews>
@@ -339,7 +339,7 @@
     <t>Description007zzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzz</t>
   </si>
   <si>
-    <t>some test textzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzz</t>
+    <t>some test textzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzz</t>
   </si>
 </sst>
 </file>
@@ -1067,7 +1067,7 @@
       </c>
       <c r="B1" s="24">
         <f>SUM(B2:B295)</f>
-        <v>9640.5950000000012</v>
+        <v>9641.7950000000001</v>
       </c>
       <c r="C1" s="25"/>
       <c r="D1" s="25" t="s">
@@ -1191,7 +1191,7 @@
         <v>36</v>
       </c>
       <c r="B9" s="27">
-        <v>1328.96</v>
+        <v>1330.16</v>
       </c>
       <c r="C9" s="28"/>
       <c r="D9" s="30" t="s">
@@ -2065,10 +2065,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>43222</v>
+        <v>43223</v>
       </c>
       <c r="B10" s="5">
-        <v>71.94</v>
+        <v>73.14</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Tinkering with record tests - trying to find out why bank records are always slower.
</commit_message>
<xml_diff>
--- a/spreadsheet-samples/Test-Spreadsheet.xlsx
+++ b/spreadsheet-samples/Test-Spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\Reconciliate\spreadsheet-samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9144FB6F-53BB-40A5-A402-CAB641F3E825}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E69E88D3-C63E-4C1B-A033-94B6745E1922}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="780" windowWidth="18000" windowHeight="9360" firstSheet="5" activeTab="9" xr2:uid="{E73E5FC3-A692-4EF9-93A1-0012994854D9}"/>
   </bookViews>
@@ -339,7 +339,7 @@
     <t>Description007zzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzz</t>
   </si>
   <si>
-    <t>some test textzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzz</t>
+    <t>some test textzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzz</t>
   </si>
 </sst>
 </file>
@@ -1067,7 +1067,7 @@
       </c>
       <c r="B1" s="24">
         <f>SUM(B2:B295)</f>
-        <v>9641.7950000000001</v>
+        <v>9650.1949999999997</v>
       </c>
       <c r="C1" s="25"/>
       <c r="D1" s="25" t="s">
@@ -1191,7 +1191,7 @@
         <v>36</v>
       </c>
       <c r="B9" s="27">
-        <v>1330.16</v>
+        <v>1338.56</v>
       </c>
       <c r="C9" s="28"/>
       <c r="D9" s="30" t="s">
@@ -2065,10 +2065,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>43223</v>
+        <v>43230</v>
       </c>
       <c r="B10" s="5">
-        <v>73.14</v>
+        <v>81.540000000000006</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
More tinkering with records to see why bank records are slower (see Slow-test-refactor-notes.txt)
</commit_message>
<xml_diff>
--- a/spreadsheet-samples/Test-Spreadsheet.xlsx
+++ b/spreadsheet-samples/Test-Spreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\Reconciliate\spreadsheet-samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E69E88D3-C63E-4C1B-A033-94B6745E1922}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DAF143C-B088-4466-A89B-9233F600D537}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="18000" windowHeight="9360" firstSheet="5" activeTab="9" xr2:uid="{E73E5FC3-A692-4EF9-93A1-0012994854D9}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="18000" windowHeight="9360" activeTab="3" xr2:uid="{E73E5FC3-A692-4EF9-93A1-0012994854D9}"/>
   </bookViews>
   <sheets>
     <sheet name="Bank" sheetId="7" r:id="rId1"/>
@@ -100,7 +100,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="80">
   <si>
     <t>Col1</t>
   </si>
@@ -339,7 +339,7 @@
     <t>Description007zzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzz</t>
   </si>
   <si>
-    <t>some test textzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzz</t>
+    <t>some test textzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzz</t>
   </si>
 </sst>
 </file>
@@ -875,7 +875,7 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4:D7"/>
+      <selection activeCell="F1" sqref="F1:J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1049,7 +1049,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEB17BBD-6FBB-4BDC-8FD6-599D29D94644}">
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
@@ -1067,7 +1067,7 @@
       </c>
       <c r="B1" s="24">
         <f>SUM(B2:B295)</f>
-        <v>9650.1949999999997</v>
+        <v>9653.7950000000001</v>
       </c>
       <c r="C1" s="25"/>
       <c r="D1" s="25" t="s">
@@ -1191,7 +1191,7 @@
         <v>36</v>
       </c>
       <c r="B9" s="27">
-        <v>1338.56</v>
+        <v>1342.16</v>
       </c>
       <c r="C9" s="28"/>
       <c r="D9" s="30" t="s">
@@ -1552,10 +1552,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8ADEDA7-CE7F-46FB-B96B-C8F28E94F278}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11:J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1564,9 +1564,10 @@
     <col min="2" max="2" width="9.140625" style="6"/>
     <col min="4" max="4" width="60.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
         <v>43210</v>
       </c>
@@ -1579,14 +1580,20 @@
       <c r="E1" s="6">
         <v>4567.8900000000003</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B2" s="14" t="s">
         <v>20</v>
       </c>
       <c r="E2" s="14"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43211</v>
       </c>
@@ -1599,8 +1606,21 @@
       <c r="E3" s="14">
         <v>4567.8900000000003</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" s="12">
+        <v>12345</v>
+      </c>
+      <c r="G3" s="15">
+        <v>4567.8900000000003</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>43212</v>
       </c>
@@ -1613,14 +1633,27 @@
       <c r="E4" s="14">
         <v>5567.89</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" s="12">
+        <v>12345</v>
+      </c>
+      <c r="G4" s="15">
+        <v>4567.8900000000003</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B5" s="14" t="s">
         <v>20</v>
       </c>
       <c r="E5" s="14"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>43213</v>
       </c>
@@ -1633,8 +1666,20 @@
       <c r="E6" s="14">
         <v>6567.89</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6" s="13">
+        <v>22345</v>
+      </c>
+      <c r="G6" s="14">
+        <v>5567.89</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="J6" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>43214</v>
       </c>
@@ -1647,8 +1692,20 @@
       <c r="E7" s="14">
         <v>7567.89</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7" s="13">
+        <v>42345</v>
+      </c>
+      <c r="G7" s="14">
+        <v>7567.89</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="J7" s="9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>43215</v>
       </c>
@@ -1659,14 +1716,26 @@
         <v>31</v>
       </c>
       <c r="E8" s="14"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8" s="13">
+        <v>42345</v>
+      </c>
+      <c r="G8" s="14">
+        <v>7567.89</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="J8" s="9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="14" t="s">
         <v>20</v>
       </c>
       <c r="E9" s="14"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>43216</v>
       </c>
@@ -1679,8 +1748,20 @@
       <c r="E10" s="14">
         <v>9567.89</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F10" s="13">
+        <v>42345</v>
+      </c>
+      <c r="G10" s="14">
+        <v>7567.89</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="J10" s="9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>43217</v>
       </c>
@@ -1692,6 +1773,18 @@
       </c>
       <c r="E11" s="14">
         <v>10567.89</v>
+      </c>
+      <c r="F11" s="13">
+        <v>42345</v>
+      </c>
+      <c r="G11" s="14">
+        <v>7567.89</v>
+      </c>
+      <c r="H11" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="J11" s="9" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -2065,10 +2158,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>43230</v>
+        <v>43233</v>
       </c>
       <c r="B10" s="5">
-        <v>81.540000000000006</v>
+        <v>85.14</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Have one central spreadsheet, used by all tests.
</commit_message>
<xml_diff>
--- a/spreadsheet-samples/Test-Spreadsheet.xlsx
+++ b/spreadsheet-samples/Test-Spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\Reconciliate\spreadsheet-samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DAF143C-B088-4466-A89B-9233F600D537}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{138C999D-2C23-45FA-A04B-E79B8A720C72}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="780" windowWidth="18000" windowHeight="9360" activeTab="3" xr2:uid="{E73E5FC3-A692-4EF9-93A1-0012994854D9}"/>
   </bookViews>
@@ -339,7 +339,7 @@
     <t>Description007zzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzz</t>
   </si>
   <si>
-    <t>some test textzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzz</t>
+    <t>some test textzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzz</t>
   </si>
 </sst>
 </file>
@@ -2158,10 +2158,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>43233</v>
+        <v>43238</v>
       </c>
       <c r="B10" s="5">
-        <v>85.14</v>
+        <v>91.14</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Ignore all the tests which use mocking.
</commit_message>
<xml_diff>
--- a/spreadsheet-samples/Test-Spreadsheet.xlsx
+++ b/spreadsheet-samples/Test-Spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\Reconciliate\spreadsheet-samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{138C999D-2C23-45FA-A04B-E79B8A720C72}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3547D244-34B0-4961-9677-8431384C6BFB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="780" windowWidth="18000" windowHeight="9360" activeTab="3" xr2:uid="{E73E5FC3-A692-4EF9-93A1-0012994854D9}"/>
   </bookViews>
@@ -339,7 +339,7 @@
     <t>Description007zzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzz</t>
   </si>
   <si>
-    <t>some test textzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzz</t>
+    <t>some test textzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzz</t>
   </si>
 </sst>
 </file>
@@ -2158,10 +2158,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>43238</v>
+        <v>43241</v>
       </c>
       <c r="B10" s="5">
-        <v>91.14</v>
+        <v>94.74</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Writing up what I've discovered so far.
</commit_message>
<xml_diff>
--- a/spreadsheet-samples/Test-Spreadsheet.xlsx
+++ b/spreadsheet-samples/Test-Spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\Reconciliate\spreadsheet-samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3547D244-34B0-4961-9677-8431384C6BFB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF7741EB-3042-4CCB-BAED-5F66BF164405}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="780" windowWidth="18000" windowHeight="9360" activeTab="3" xr2:uid="{E73E5FC3-A692-4EF9-93A1-0012994854D9}"/>
   </bookViews>
@@ -339,7 +339,7 @@
     <t>Description007zzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzz</t>
   </si>
   <si>
-    <t>some test textzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzz</t>
+    <t>some test textzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzz</t>
   </si>
 </sst>
 </file>
@@ -2158,10 +2158,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>43241</v>
+        <v>43245</v>
       </c>
       <c r="B10" s="5">
-        <v>94.74</v>
+        <v>99.54</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Moved a bunch of slow reconciliation tests into a separate test project so they could be run in parallel.
</commit_message>
<xml_diff>
--- a/spreadsheet-samples/Test-Spreadsheet.xlsx
+++ b/spreadsheet-samples/Test-Spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\Reconciliate\spreadsheet-samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF7741EB-3042-4CCB-BAED-5F66BF164405}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3D5D771-916C-46EF-A0FC-C2EBCDA4A21B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="780" windowWidth="18000" windowHeight="9360" activeTab="3" xr2:uid="{E73E5FC3-A692-4EF9-93A1-0012994854D9}"/>
   </bookViews>
@@ -339,7 +339,7 @@
     <t>Description007zzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzz</t>
   </si>
   <si>
-    <t>some test textzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzz</t>
+    <t>some test textzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzz</t>
   </si>
 </sst>
 </file>
@@ -2158,10 +2158,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>43245</v>
+        <v>43252</v>
       </c>
       <c r="B10" s="5">
-        <v>99.54</v>
+        <v>107.94</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Rename ReconciliationIntegrationTests => ReconciliationBaseTests
</commit_message>
<xml_diff>
--- a/spreadsheet-samples/Test-Spreadsheet.xlsx
+++ b/spreadsheet-samples/Test-Spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\Reconciliate\spreadsheet-samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3D5D771-916C-46EF-A0FC-C2EBCDA4A21B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB23F5D0-8EE3-4623-A935-829EFB3B212A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="780" windowWidth="18000" windowHeight="9360" activeTab="3" xr2:uid="{E73E5FC3-A692-4EF9-93A1-0012994854D9}"/>
   </bookViews>
@@ -339,7 +339,7 @@
     <t>Description007zzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzz</t>
   </si>
   <si>
-    <t>some test textzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzz</t>
+    <t>some test textzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzz</t>
   </si>
 </sst>
 </file>
@@ -2158,10 +2158,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>43252</v>
+        <v>43258</v>
       </c>
       <c r="B10" s="5">
-        <v>107.94</v>
+        <v>115.14</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Reinstate ignored Excel integration tests, and had to stop sharing spreadsheet across two test files (because it didn't work with the previously-ignored tests).
</commit_message>
<xml_diff>
--- a/spreadsheet-samples/Test-Spreadsheet.xlsx
+++ b/spreadsheet-samples/Test-Spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\Reconciliate\spreadsheet-samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB23F5D0-8EE3-4623-A935-829EFB3B212A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FB56F0C-B16B-4A9F-A24C-711E70ED20D6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="780" windowWidth="18000" windowHeight="9360" activeTab="3" xr2:uid="{E73E5FC3-A692-4EF9-93A1-0012994854D9}"/>
   </bookViews>
@@ -336,10 +336,10 @@
     <t>ABC</t>
   </si>
   <si>
-    <t>Description007zzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzz</t>
-  </si>
-  <si>
-    <t>some test textzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzz</t>
+    <t>Description007zzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzz</t>
+  </si>
+  <si>
+    <t>some test textzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzz</t>
   </si>
 </sst>
 </file>
@@ -1067,7 +1067,7 @@
       </c>
       <c r="B1" s="24">
         <f>SUM(B2:B295)</f>
-        <v>9653.7950000000001</v>
+        <v>9660.994999999999</v>
       </c>
       <c r="C1" s="25"/>
       <c r="D1" s="25" t="s">
@@ -1191,7 +1191,7 @@
         <v>36</v>
       </c>
       <c r="B9" s="27">
-        <v>1342.16</v>
+        <v>1345.76</v>
       </c>
       <c r="C9" s="28"/>
       <c r="D9" s="30" t="s">
@@ -1223,7 +1223,7 @@
         <v>37</v>
       </c>
       <c r="B11" s="27">
-        <v>422.02</v>
+        <v>425.62</v>
       </c>
       <c r="C11" s="28"/>
       <c r="D11" s="30" t="s">
@@ -2158,10 +2158,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>43258</v>
+        <v>43261</v>
       </c>
       <c r="B10" s="5">
-        <v>115.14</v>
+        <v>118.74</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
@@ -2482,7 +2482,7 @@
         <v>43405</v>
       </c>
       <c r="C9" s="19">
-        <v>84.22</v>
+        <v>87.82</v>
       </c>
       <c r="D9" s="19"/>
       <c r="E9" s="21" t="s">

</xml_diff>

<commit_message>
Moved first method from FileLoader back into ReconciliationIntro
</commit_message>
<xml_diff>
--- a/spreadsheet-samples/Test-Spreadsheet.xlsx
+++ b/spreadsheet-samples/Test-Spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\Reconciliate\spreadsheet-samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FB56F0C-B16B-4A9F-A24C-711E70ED20D6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F14BDE7-7BF5-42C6-8548-30EC7BA0AED7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="780" windowWidth="18000" windowHeight="9360" activeTab="3" xr2:uid="{E73E5FC3-A692-4EF9-93A1-0012994854D9}"/>
   </bookViews>
@@ -336,10 +336,10 @@
     <t>ABC</t>
   </si>
   <si>
-    <t>Description007zzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzz</t>
-  </si>
-  <si>
-    <t>some test textzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzz</t>
+    <t>Description007zzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzz</t>
+  </si>
+  <si>
+    <t>some test textzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzz</t>
   </si>
 </sst>
 </file>
@@ -1067,7 +1067,7 @@
       </c>
       <c r="B1" s="24">
         <f>SUM(B2:B295)</f>
-        <v>9660.994999999999</v>
+        <v>9663.3950000000004</v>
       </c>
       <c r="C1" s="25"/>
       <c r="D1" s="25" t="s">
@@ -1191,7 +1191,7 @@
         <v>36</v>
       </c>
       <c r="B9" s="27">
-        <v>1345.76</v>
+        <v>1346.96</v>
       </c>
       <c r="C9" s="28"/>
       <c r="D9" s="30" t="s">
@@ -1223,7 +1223,7 @@
         <v>37</v>
       </c>
       <c r="B11" s="27">
-        <v>425.62</v>
+        <v>426.82</v>
       </c>
       <c r="C11" s="28"/>
       <c r="D11" s="30" t="s">
@@ -2158,10 +2158,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>43261</v>
+        <v>43262</v>
       </c>
       <c r="B10" s="5">
-        <v>118.74</v>
+        <v>119.94</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
@@ -2482,7 +2482,7 @@
         <v>43405</v>
       </c>
       <c r="C9" s="19">
-        <v>87.82</v>
+        <v>89.02</v>
       </c>
       <c r="D9" s="19"/>
       <c r="E9" s="21" t="s">

</xml_diff>

<commit_message>
BankAndBankInMatcher mpt using passed in IBankAndBankInLoader any more.
</commit_message>
<xml_diff>
--- a/spreadsheet-samples/Test-Spreadsheet.xlsx
+++ b/spreadsheet-samples/Test-Spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\Reconciliate\spreadsheet-samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F14BDE7-7BF5-42C6-8548-30EC7BA0AED7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2960474F-F5BC-4186-BDF1-7A59A66FBE84}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="780" windowWidth="18000" windowHeight="9360" activeTab="3" xr2:uid="{E73E5FC3-A692-4EF9-93A1-0012994854D9}"/>
   </bookViews>
@@ -336,10 +336,10 @@
     <t>ABC</t>
   </si>
   <si>
-    <t>Description007zzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzz</t>
-  </si>
-  <si>
-    <t>some test textzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzz</t>
+    <t>Description007zzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzz</t>
+  </si>
+  <si>
+    <t>some test textzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzz</t>
   </si>
 </sst>
 </file>
@@ -1067,7 +1067,7 @@
       </c>
       <c r="B1" s="24">
         <f>SUM(B2:B295)</f>
-        <v>9663.3950000000004</v>
+        <v>9665.7950000000001</v>
       </c>
       <c r="C1" s="25"/>
       <c r="D1" s="25" t="s">
@@ -1191,7 +1191,7 @@
         <v>36</v>
       </c>
       <c r="B9" s="27">
-        <v>1346.96</v>
+        <v>1348.16</v>
       </c>
       <c r="C9" s="28"/>
       <c r="D9" s="30" t="s">
@@ -1223,7 +1223,7 @@
         <v>37</v>
       </c>
       <c r="B11" s="27">
-        <v>426.82</v>
+        <v>428.02</v>
       </c>
       <c r="C11" s="28"/>
       <c r="D11" s="30" t="s">
@@ -2158,10 +2158,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>43262</v>
+        <v>43263</v>
       </c>
       <c r="B10" s="5">
-        <v>119.94</v>
+        <v>121.14</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
@@ -2482,7 +2482,7 @@
         <v>43405</v>
       </c>
       <c r="C9" s="19">
-        <v>89.02</v>
+        <v>90.22</v>
       </c>
       <c r="D9" s="19"/>
       <c r="E9" s="21" t="s">

</xml_diff>

<commit_message>
Added some new debugging files, for manual testing. Also added/updated instructions.
</commit_message>
<xml_diff>
--- a/spreadsheet-samples/Test-Spreadsheet.xlsx
+++ b/spreadsheet-samples/Test-Spreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\Reconciliate\spreadsheet-samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2960474F-F5BC-4186-BDF1-7A59A66FBE84}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{604ABB1C-6FAA-4529-83CE-1E7E73A95A45}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="18000" windowHeight="9360" activeTab="3" xr2:uid="{E73E5FC3-A692-4EF9-93A1-0012994854D9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="3" xr2:uid="{E73E5FC3-A692-4EF9-93A1-0012994854D9}"/>
   </bookViews>
   <sheets>
     <sheet name="Bank" sheetId="7" r:id="rId1"/>
@@ -100,7 +100,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="80">
   <si>
     <t>Col1</t>
   </si>
@@ -1555,7 +1555,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11:J11"/>
+      <selection activeCell="F1" sqref="F1:J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1580,12 +1580,8 @@
       <c r="E1" s="6">
         <v>4567.8900000000003</v>
       </c>
-      <c r="F1" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="G1" s="14" t="s">
-        <v>15</v>
-      </c>
+      <c r="F1" s="13"/>
+      <c r="G1" s="14"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B2" s="14" t="s">
@@ -1606,19 +1602,11 @@
       <c r="E3" s="14">
         <v>4567.8900000000003</v>
       </c>
-      <c r="F3" s="12">
-        <v>12345</v>
-      </c>
-      <c r="G3" s="15">
-        <v>4567.8900000000003</v>
-      </c>
-      <c r="H3" s="9" t="s">
-        <v>7</v>
-      </c>
+      <c r="F3" s="12"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="9"/>
       <c r="I3" s="9"/>
-      <c r="J3" s="9" t="s">
-        <v>8</v>
-      </c>
+      <c r="J3" s="9"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
@@ -1633,19 +1621,11 @@
       <c r="E4" s="14">
         <v>5567.89</v>
       </c>
-      <c r="F4" s="12">
-        <v>12345</v>
-      </c>
-      <c r="G4" s="15">
-        <v>4567.8900000000003</v>
-      </c>
-      <c r="H4" s="9" t="s">
-        <v>22</v>
-      </c>
+      <c r="F4" s="12"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="9"/>
       <c r="I4" s="9"/>
-      <c r="J4" s="9" t="s">
-        <v>23</v>
-      </c>
+      <c r="J4" s="9"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B5" s="14" t="s">
@@ -1666,18 +1646,10 @@
       <c r="E6" s="14">
         <v>6567.89</v>
       </c>
-      <c r="F6" s="13">
-        <v>22345</v>
-      </c>
-      <c r="G6" s="14">
-        <v>5567.89</v>
-      </c>
-      <c r="H6" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="J6" s="9" t="s">
-        <v>26</v>
-      </c>
+      <c r="F6" s="13"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="9"/>
+      <c r="J6" s="9"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
@@ -1692,18 +1664,10 @@
       <c r="E7" s="14">
         <v>7567.89</v>
       </c>
-      <c r="F7" s="13">
-        <v>42345</v>
-      </c>
-      <c r="G7" s="14">
-        <v>7567.89</v>
-      </c>
-      <c r="H7" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="J7" s="9" t="s">
-        <v>30</v>
-      </c>
+      <c r="F7" s="13"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="9"/>
+      <c r="J7" s="9"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
@@ -1716,18 +1680,10 @@
         <v>31</v>
       </c>
       <c r="E8" s="14"/>
-      <c r="F8" s="13">
-        <v>42345</v>
-      </c>
-      <c r="G8" s="14">
-        <v>7567.89</v>
-      </c>
-      <c r="H8" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="J8" s="9" t="s">
-        <v>30</v>
-      </c>
+      <c r="F8" s="13"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="9"/>
+      <c r="J8" s="9"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="14" t="s">
@@ -1748,18 +1704,10 @@
       <c r="E10" s="14">
         <v>9567.89</v>
       </c>
-      <c r="F10" s="13">
-        <v>42345</v>
-      </c>
-      <c r="G10" s="14">
-        <v>7567.89</v>
-      </c>
-      <c r="H10" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="J10" s="9" t="s">
-        <v>30</v>
-      </c>
+      <c r="F10" s="13"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="9"/>
+      <c r="J10" s="9"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
@@ -1774,18 +1722,10 @@
       <c r="E11" s="14">
         <v>10567.89</v>
       </c>
-      <c r="F11" s="13">
-        <v>42345</v>
-      </c>
-      <c r="G11" s="14">
-        <v>7567.89</v>
-      </c>
-      <c r="H11" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="J11" s="9" t="s">
-        <v>30</v>
-      </c>
+      <c r="F11" s="13"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="9"/>
+      <c r="J11" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added some new debugging files, for manual testing. Also added/updated instructions (copied over from Refactor-eg-genericise branch, commit c08d46e).
</commit_message>
<xml_diff>
--- a/spreadsheet-samples/Test-Spreadsheet.xlsx
+++ b/spreadsheet-samples/Test-Spreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\Reconciliate\spreadsheet-samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FB56F0C-B16B-4A9F-A24C-711E70ED20D6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{604ABB1C-6FAA-4529-83CE-1E7E73A95A45}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="18000" windowHeight="9360" activeTab="3" xr2:uid="{E73E5FC3-A692-4EF9-93A1-0012994854D9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="3" xr2:uid="{E73E5FC3-A692-4EF9-93A1-0012994854D9}"/>
   </bookViews>
   <sheets>
     <sheet name="Bank" sheetId="7" r:id="rId1"/>
@@ -100,7 +100,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="80">
   <si>
     <t>Col1</t>
   </si>
@@ -336,10 +336,10 @@
     <t>ABC</t>
   </si>
   <si>
-    <t>Description007zzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzz</t>
-  </si>
-  <si>
-    <t>some test textzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzz</t>
+    <t>Description007zzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzz</t>
+  </si>
+  <si>
+    <t>some test textzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzz</t>
   </si>
 </sst>
 </file>
@@ -1067,7 +1067,7 @@
       </c>
       <c r="B1" s="24">
         <f>SUM(B2:B295)</f>
-        <v>9660.994999999999</v>
+        <v>9665.7950000000001</v>
       </c>
       <c r="C1" s="25"/>
       <c r="D1" s="25" t="s">
@@ -1191,7 +1191,7 @@
         <v>36</v>
       </c>
       <c r="B9" s="27">
-        <v>1345.76</v>
+        <v>1348.16</v>
       </c>
       <c r="C9" s="28"/>
       <c r="D9" s="30" t="s">
@@ -1223,7 +1223,7 @@
         <v>37</v>
       </c>
       <c r="B11" s="27">
-        <v>425.62</v>
+        <v>428.02</v>
       </c>
       <c r="C11" s="28"/>
       <c r="D11" s="30" t="s">
@@ -1555,7 +1555,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11:J11"/>
+      <selection activeCell="F1" sqref="F1:J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1580,12 +1580,8 @@
       <c r="E1" s="6">
         <v>4567.8900000000003</v>
       </c>
-      <c r="F1" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="G1" s="14" t="s">
-        <v>15</v>
-      </c>
+      <c r="F1" s="13"/>
+      <c r="G1" s="14"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B2" s="14" t="s">
@@ -1606,19 +1602,11 @@
       <c r="E3" s="14">
         <v>4567.8900000000003</v>
       </c>
-      <c r="F3" s="12">
-        <v>12345</v>
-      </c>
-      <c r="G3" s="15">
-        <v>4567.8900000000003</v>
-      </c>
-      <c r="H3" s="9" t="s">
-        <v>7</v>
-      </c>
+      <c r="F3" s="12"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="9"/>
       <c r="I3" s="9"/>
-      <c r="J3" s="9" t="s">
-        <v>8</v>
-      </c>
+      <c r="J3" s="9"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
@@ -1633,19 +1621,11 @@
       <c r="E4" s="14">
         <v>5567.89</v>
       </c>
-      <c r="F4" s="12">
-        <v>12345</v>
-      </c>
-      <c r="G4" s="15">
-        <v>4567.8900000000003</v>
-      </c>
-      <c r="H4" s="9" t="s">
-        <v>22</v>
-      </c>
+      <c r="F4" s="12"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="9"/>
       <c r="I4" s="9"/>
-      <c r="J4" s="9" t="s">
-        <v>23</v>
-      </c>
+      <c r="J4" s="9"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B5" s="14" t="s">
@@ -1666,18 +1646,10 @@
       <c r="E6" s="14">
         <v>6567.89</v>
       </c>
-      <c r="F6" s="13">
-        <v>22345</v>
-      </c>
-      <c r="G6" s="14">
-        <v>5567.89</v>
-      </c>
-      <c r="H6" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="J6" s="9" t="s">
-        <v>26</v>
-      </c>
+      <c r="F6" s="13"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="9"/>
+      <c r="J6" s="9"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
@@ -1692,18 +1664,10 @@
       <c r="E7" s="14">
         <v>7567.89</v>
       </c>
-      <c r="F7" s="13">
-        <v>42345</v>
-      </c>
-      <c r="G7" s="14">
-        <v>7567.89</v>
-      </c>
-      <c r="H7" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="J7" s="9" t="s">
-        <v>30</v>
-      </c>
+      <c r="F7" s="13"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="9"/>
+      <c r="J7" s="9"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
@@ -1716,18 +1680,10 @@
         <v>31</v>
       </c>
       <c r="E8" s="14"/>
-      <c r="F8" s="13">
-        <v>42345</v>
-      </c>
-      <c r="G8" s="14">
-        <v>7567.89</v>
-      </c>
-      <c r="H8" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="J8" s="9" t="s">
-        <v>30</v>
-      </c>
+      <c r="F8" s="13"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="9"/>
+      <c r="J8" s="9"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="14" t="s">
@@ -1748,18 +1704,10 @@
       <c r="E10" s="14">
         <v>9567.89</v>
       </c>
-      <c r="F10" s="13">
-        <v>42345</v>
-      </c>
-      <c r="G10" s="14">
-        <v>7567.89</v>
-      </c>
-      <c r="H10" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="J10" s="9" t="s">
-        <v>30</v>
-      </c>
+      <c r="F10" s="13"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="9"/>
+      <c r="J10" s="9"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
@@ -1774,18 +1722,10 @@
       <c r="E11" s="14">
         <v>10567.89</v>
       </c>
-      <c r="F11" s="13">
-        <v>42345</v>
-      </c>
-      <c r="G11" s="14">
-        <v>7567.89</v>
-      </c>
-      <c r="H11" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="J11" s="9" t="s">
-        <v>30</v>
-      </c>
+      <c r="F11" s="13"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="9"/>
+      <c r="J11" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2158,10 +2098,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>43261</v>
+        <v>43263</v>
       </c>
       <c r="B10" s="5">
-        <v>118.74</v>
+        <v>121.14</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
@@ -2482,7 +2422,7 @@
         <v>43405</v>
       </c>
       <c r="C9" s="19">
-        <v>87.82</v>
+        <v>90.22</v>
       </c>
       <c r="D9" s="19"/>
       <c r="E9" s="21" t="s">

</xml_diff>

<commit_message>
Fixed bug of reconciliaiton type getting reset, and bug of pending file not having paths set. also removed some unnecessary type-specific methods.
</commit_message>
<xml_diff>
--- a/spreadsheet-samples/Test-Spreadsheet.xlsx
+++ b/spreadsheet-samples/Test-Spreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\Reconciliate\spreadsheet-samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{604ABB1C-6FAA-4529-83CE-1E7E73A95A45}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D920362-2533-481A-AA02-DE2DE0BA93BC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="3" xr2:uid="{E73E5FC3-A692-4EF9-93A1-0012994854D9}"/>
+    <workbookView xWindow="-18975" yWindow="1710" windowWidth="18000" windowHeight="9360" activeTab="3" xr2:uid="{E73E5FC3-A692-4EF9-93A1-0012994854D9}"/>
   </bookViews>
   <sheets>
     <sheet name="Bank" sheetId="7" r:id="rId1"/>
@@ -336,10 +336,10 @@
     <t>ABC</t>
   </si>
   <si>
-    <t>Description007zzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzz</t>
-  </si>
-  <si>
-    <t>some test textzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzz</t>
+    <t>Description007zzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzz</t>
+  </si>
+  <si>
+    <t>some test textzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzz</t>
   </si>
 </sst>
 </file>
@@ -1067,7 +1067,7 @@
       </c>
       <c r="B1" s="24">
         <f>SUM(B2:B295)</f>
-        <v>9665.7950000000001</v>
+        <v>9670.5950000000012</v>
       </c>
       <c r="C1" s="25"/>
       <c r="D1" s="25" t="s">
@@ -1191,7 +1191,7 @@
         <v>36</v>
       </c>
       <c r="B9" s="27">
-        <v>1348.16</v>
+        <v>1350.56</v>
       </c>
       <c r="C9" s="28"/>
       <c r="D9" s="30" t="s">
@@ -1223,7 +1223,7 @@
         <v>37</v>
       </c>
       <c r="B11" s="27">
-        <v>428.02</v>
+        <v>430.42</v>
       </c>
       <c r="C11" s="28"/>
       <c r="D11" s="30" t="s">
@@ -2098,10 +2098,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>43263</v>
+        <v>43265</v>
       </c>
       <c r="B10" s="5">
-        <v>121.14</v>
+        <v>123.54</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
@@ -2422,7 +2422,7 @@
         <v>43405</v>
       </c>
       <c r="C9" s="19">
-        <v>90.22</v>
+        <v>92.62</v>
       </c>
       <c r="D9" s="19"/>
       <c r="E9" s="21" t="s">

</xml_diff>

<commit_message>
Rearranged ReconciliationIntro methods into regions, so we can see where the different class responsibilities lie.
</commit_message>
<xml_diff>
--- a/spreadsheet-samples/Test-Spreadsheet.xlsx
+++ b/spreadsheet-samples/Test-Spreadsheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\Reconciliate\spreadsheet-samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D920362-2533-481A-AA02-DE2DE0BA93BC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE1CD677-B4D3-41D1-A895-5232F245C01F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-18975" yWindow="1710" windowWidth="18000" windowHeight="9360" activeTab="3" xr2:uid="{E73E5FC3-A692-4EF9-93A1-0012994854D9}"/>
+    <workbookView xWindow="24735" yWindow="1275" windowWidth="18000" windowHeight="9360" activeTab="3" xr2:uid="{E73E5FC3-A692-4EF9-93A1-0012994854D9}"/>
   </bookViews>
   <sheets>
     <sheet name="Bank" sheetId="7" r:id="rId1"/>
@@ -336,10 +336,10 @@
     <t>ABC</t>
   </si>
   <si>
-    <t>Description007zzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzz</t>
-  </si>
-  <si>
-    <t>some test textzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzz</t>
+    <t>Description007zzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzz</t>
+  </si>
+  <si>
+    <t>some test textzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzz</t>
   </si>
 </sst>
 </file>
@@ -1067,7 +1067,7 @@
       </c>
       <c r="B1" s="24">
         <f>SUM(B2:B295)</f>
-        <v>9670.5950000000012</v>
+        <v>9672.994999999999</v>
       </c>
       <c r="C1" s="25"/>
       <c r="D1" s="25" t="s">
@@ -1191,7 +1191,7 @@
         <v>36</v>
       </c>
       <c r="B9" s="27">
-        <v>1350.56</v>
+        <v>1351.76</v>
       </c>
       <c r="C9" s="28"/>
       <c r="D9" s="30" t="s">
@@ -1223,7 +1223,7 @@
         <v>37</v>
       </c>
       <c r="B11" s="27">
-        <v>430.42</v>
+        <v>431.62</v>
       </c>
       <c r="C11" s="28"/>
       <c r="D11" s="30" t="s">
@@ -2098,10 +2098,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>43265</v>
+        <v>43266</v>
       </c>
       <c r="B10" s="5">
-        <v>123.54</v>
+        <v>124.74</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
@@ -2422,7 +2422,7 @@
         <v>43405</v>
       </c>
       <c r="C9" s="19">
-        <v>92.62</v>
+        <v>93.82</v>
       </c>
       <c r="D9" s="19"/>
       <c r="E9" s="21" t="s">

</xml_diff>

<commit_message>
Rename refactor: Use snake_case on all local variables
</commit_message>
<xml_diff>
--- a/spreadsheet-samples/Test-Spreadsheet.xlsx
+++ b/spreadsheet-samples/Test-Spreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\Reconciliate\spreadsheet-samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE1CD677-B4D3-41D1-A895-5232F245C01F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6DB829A-5FA6-4500-B01F-D96B7A05A702}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24735" yWindow="1275" windowWidth="18000" windowHeight="9360" activeTab="3" xr2:uid="{E73E5FC3-A692-4EF9-93A1-0012994854D9}"/>
+    <workbookView xWindow="24735" yWindow="1275" windowWidth="18000" windowHeight="10800" activeTab="3" xr2:uid="{E73E5FC3-A692-4EF9-93A1-0012994854D9}"/>
   </bookViews>
   <sheets>
     <sheet name="Bank" sheetId="7" r:id="rId1"/>
@@ -336,10 +336,10 @@
     <t>ABC</t>
   </si>
   <si>
-    <t>Description007zzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzz</t>
-  </si>
-  <si>
-    <t>some test textzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzz</t>
+    <t>Description007zzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzz</t>
+  </si>
+  <si>
+    <t>some test textzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzz</t>
   </si>
 </sst>
 </file>
@@ -1067,7 +1067,7 @@
       </c>
       <c r="B1" s="24">
         <f>SUM(B2:B295)</f>
-        <v>9672.994999999999</v>
+        <v>9677.7950000000001</v>
       </c>
       <c r="C1" s="25"/>
       <c r="D1" s="25" t="s">
@@ -1191,7 +1191,7 @@
         <v>36</v>
       </c>
       <c r="B9" s="27">
-        <v>1351.76</v>
+        <v>1354.16</v>
       </c>
       <c r="C9" s="28"/>
       <c r="D9" s="30" t="s">
@@ -1223,7 +1223,7 @@
         <v>37</v>
       </c>
       <c r="B11" s="27">
-        <v>431.62</v>
+        <v>434.02</v>
       </c>
       <c r="C11" s="28"/>
       <c r="D11" s="30" t="s">
@@ -2098,10 +2098,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>43266</v>
+        <v>43268</v>
       </c>
       <c r="B10" s="5">
-        <v>124.74</v>
+        <v>127.14</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
@@ -2422,7 +2422,7 @@
         <v>43405</v>
       </c>
       <c r="C9" s="19">
-        <v>93.82</v>
+        <v>96.22</v>
       </c>
       <c r="D9" s="19"/>
       <c r="E9" s="21" t="s">

</xml_diff>

<commit_message>
Fixed broken config names introduced in previous refactor
</commit_message>
<xml_diff>
--- a/spreadsheet-samples/Test-Spreadsheet.xlsx
+++ b/spreadsheet-samples/Test-Spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\Reconciliate\spreadsheet-samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8202AFC-0339-4ED7-B047-90DD45AAA551}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CE6C224-B787-4ABB-B46B-3121CEEECAF8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="24735" yWindow="1275" windowWidth="18000" windowHeight="10800" activeTab="3" xr2:uid="{E73E5FC3-A692-4EF9-93A1-0012994854D9}"/>
   </bookViews>
@@ -336,10 +336,10 @@
     <t>ABC</t>
   </si>
   <si>
-    <t>Description007zzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzz</t>
-  </si>
-  <si>
-    <t>some test textzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzz</t>
+    <t>Description007zzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzz</t>
+  </si>
+  <si>
+    <t>some test textzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzz</t>
   </si>
 </sst>
 </file>
@@ -1067,7 +1067,7 @@
       </c>
       <c r="B1" s="24">
         <f>SUM(B2:B295)</f>
-        <v>9677.7950000000001</v>
+        <v>9680.1949999999997</v>
       </c>
       <c r="C1" s="25"/>
       <c r="D1" s="25" t="s">
@@ -1191,7 +1191,7 @@
         <v>36</v>
       </c>
       <c r="B9" s="27">
-        <v>1354.16</v>
+        <v>1355.36</v>
       </c>
       <c r="C9" s="28"/>
       <c r="D9" s="30" t="s">
@@ -1223,7 +1223,7 @@
         <v>37</v>
       </c>
       <c r="B11" s="27">
-        <v>434.02</v>
+        <v>435.22</v>
       </c>
       <c r="C11" s="28"/>
       <c r="D11" s="30" t="s">
@@ -2098,10 +2098,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>43268</v>
+        <v>43269</v>
       </c>
       <c r="B10" s="5">
-        <v>127.14</v>
+        <v>128.34</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
@@ -2422,7 +2422,7 @@
         <v>43405</v>
       </c>
       <c r="C9" s="19">
-        <v>96.22</v>
+        <v>97.42</v>
       </c>
       <c r="D9" s="19"/>
       <c r="E9" s="21" t="s">

</xml_diff>

<commit_message>
Rename refactor: Intfroduce snake_case to member variables.
</commit_message>
<xml_diff>
--- a/spreadsheet-samples/Test-Spreadsheet.xlsx
+++ b/spreadsheet-samples/Test-Spreadsheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\Reconciliate\spreadsheet-samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CE6C224-B787-4ABB-B46B-3121CEEECAF8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F7FA9CF-4753-47FE-AF1B-750CB1DE69B4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="24735" yWindow="1275" windowWidth="18000" windowHeight="10800" activeTab="3" xr2:uid="{E73E5FC3-A692-4EF9-93A1-0012994854D9}"/>
   </bookViews>
@@ -336,10 +336,10 @@
     <t>ABC</t>
   </si>
   <si>
-    <t>Description007zzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzz</t>
-  </si>
-  <si>
-    <t>some test textzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzz</t>
+    <t>Description007zzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzz</t>
+  </si>
+  <si>
+    <t>some test textzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzz</t>
   </si>
 </sst>
 </file>
@@ -1067,7 +1067,7 @@
       </c>
       <c r="B1" s="24">
         <f>SUM(B2:B295)</f>
-        <v>9680.1949999999997</v>
+        <v>9682.5950000000012</v>
       </c>
       <c r="C1" s="25"/>
       <c r="D1" s="25" t="s">
@@ -1191,7 +1191,7 @@
         <v>36</v>
       </c>
       <c r="B9" s="27">
-        <v>1355.36</v>
+        <v>1356.56</v>
       </c>
       <c r="C9" s="28"/>
       <c r="D9" s="30" t="s">
@@ -1223,7 +1223,7 @@
         <v>37</v>
       </c>
       <c r="B11" s="27">
-        <v>435.22</v>
+        <v>436.42</v>
       </c>
       <c r="C11" s="28"/>
       <c r="D11" s="30" t="s">
@@ -2098,10 +2098,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>43269</v>
+        <v>43270</v>
       </c>
       <c r="B10" s="5">
-        <v>128.34</v>
+        <v>129.54</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
@@ -2422,7 +2422,7 @@
         <v>43405</v>
       </c>
       <c r="C9" s="19">
-        <v>97.42</v>
+        <v>98.62</v>
       </c>
       <c r="D9" s="19"/>
       <c r="E9" s="21" t="s">

</xml_diff>

<commit_message>
Fixed build errors caused by Resharper missing some replacements when doing a rename refactor, and weird names chosen by Resharper.
</commit_message>
<xml_diff>
--- a/spreadsheet-samples/Test-Spreadsheet.xlsx
+++ b/spreadsheet-samples/Test-Spreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\Reconciliate\spreadsheet-samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A18D45C-51E7-43B7-B599-BC083FFB756E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05E848D2-F9A0-421C-88D9-C76B2D1A793B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24735" yWindow="1275" windowWidth="18000" windowHeight="9360" activeTab="3" xr2:uid="{E73E5FC3-A692-4EF9-93A1-0012994854D9}"/>
+    <workbookView xWindow="24735" yWindow="1275" windowWidth="18000" windowHeight="10800" activeTab="3" xr2:uid="{E73E5FC3-A692-4EF9-93A1-0012994854D9}"/>
   </bookViews>
   <sheets>
     <sheet name="Bank" sheetId="7" r:id="rId1"/>
@@ -336,10 +336,10 @@
     <t>ABC</t>
   </si>
   <si>
-    <t>Description007zzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzz</t>
-  </si>
-  <si>
-    <t>some test textzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzz</t>
+    <t>Description007zzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzz</t>
+  </si>
+  <si>
+    <t>some test textzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzz</t>
   </si>
 </sst>
 </file>
@@ -1067,7 +1067,7 @@
       </c>
       <c r="B1" s="24">
         <f>SUM(B2:B295)</f>
-        <v>9668.1949999999997</v>
+        <v>9672.994999999999</v>
       </c>
       <c r="C1" s="25"/>
       <c r="D1" s="25" t="s">
@@ -1191,7 +1191,7 @@
         <v>36</v>
       </c>
       <c r="B9" s="27">
-        <v>1349.36</v>
+        <v>1351.76</v>
       </c>
       <c r="C9" s="28"/>
       <c r="D9" s="30" t="s">
@@ -1223,7 +1223,7 @@
         <v>37</v>
       </c>
       <c r="B11" s="27">
-        <v>429.22</v>
+        <v>431.62</v>
       </c>
       <c r="C11" s="28"/>
       <c r="D11" s="30" t="s">
@@ -2098,10 +2098,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>43264</v>
+        <v>43266</v>
       </c>
       <c r="B10" s="5">
-        <v>122.34</v>
+        <v>124.74</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
@@ -2422,7 +2422,7 @@
         <v>43405</v>
       </c>
       <c r="C9" s="19">
-        <v>91.42</v>
+        <v>93.82</v>
       </c>
       <c r="D9" s="19"/>
       <c r="E9" s="21" t="s">

</xml_diff>

<commit_message>
Add more test data for expense matching.
</commit_message>
<xml_diff>
--- a/spreadsheet-samples/Test-Spreadsheet.xlsx
+++ b/spreadsheet-samples/Test-Spreadsheet.xlsx
@@ -1,31 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\Reconciliate\spreadsheet-samples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\development\Reconciliate\spreadsheet-samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05E848D2-F9A0-421C-88D9-C76B2D1A793B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C9859E7-665E-41DD-ADC6-194F8C9B4EBC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24735" yWindow="1275" windowWidth="18000" windowHeight="10800" activeTab="3" xr2:uid="{E73E5FC3-A692-4EF9-93A1-0012994854D9}"/>
+    <workbookView xWindow="75" yWindow="225" windowWidth="22905" windowHeight="12285" firstSheet="5" activeTab="10" xr2:uid="{E73E5FC3-A692-4EF9-93A1-0012994854D9}"/>
   </bookViews>
   <sheets>
     <sheet name="Bank" sheetId="7" r:id="rId1"/>
     <sheet name="ActualBank" sheetId="2" r:id="rId2"/>
     <sheet name="CredCard1" sheetId="6" r:id="rId3"/>
     <sheet name="CredCard" sheetId="3" r:id="rId4"/>
-    <sheet name="ForDeletingUnreconciled" sheetId="9" r:id="rId5"/>
-    <sheet name="BadDivider" sheetId="8" r:id="rId6"/>
-    <sheet name="TestRecord" sheetId="1" r:id="rId7"/>
-    <sheet name="CredCard2" sheetId="5" r:id="rId8"/>
-    <sheet name="Budget Out" sheetId="4" r:id="rId9"/>
-    <sheet name="Expected Out" sheetId="10" r:id="rId10"/>
+    <sheet name="Expected In" sheetId="11" r:id="rId5"/>
+    <sheet name="Expected Out" sheetId="10" r:id="rId6"/>
+    <sheet name="ForDeletingUnreconciled" sheetId="9" r:id="rId7"/>
+    <sheet name="BadDivider" sheetId="8" r:id="rId8"/>
+    <sheet name="TestRecord" sheetId="1" r:id="rId9"/>
+    <sheet name="CredCard2" sheetId="5" r:id="rId10"/>
+    <sheet name="Budget In" sheetId="12" r:id="rId11"/>
+    <sheet name="Budget Out" sheetId="4" r:id="rId12"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId11"/>
+    <externalReference r:id="rId13"/>
   </externalReferences>
   <definedNames>
     <definedName name="Actual_Gross">#REF!</definedName>
@@ -84,7 +86,7 @@
     <definedName name="VATRate">#REF!</definedName>
     <definedName name="VATRateToHMRC">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -92,7 +94,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -100,7 +104,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="96">
   <si>
     <t>Col1</t>
   </si>
@@ -340,6 +344,54 @@
   </si>
   <si>
     <t>some test textzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzzz</t>
+  </si>
+  <si>
+    <t>Amt (unreconciled)</t>
+  </si>
+  <si>
+    <t>Reconciled</t>
+  </si>
+  <si>
+    <t>Date paid</t>
+  </si>
+  <si>
+    <t>Total paid</t>
+  </si>
+  <si>
+    <t>already reconciled</t>
+  </si>
+  <si>
+    <t>ACME LTD - first expense</t>
+  </si>
+  <si>
+    <t>ACME LTD - second expense</t>
+  </si>
+  <si>
+    <t>ACME LTD - third expense</t>
+  </si>
+  <si>
+    <t>ACME LTD - fourth expense</t>
+  </si>
+  <si>
+    <t>ACME LTD - fifth expense</t>
+  </si>
+  <si>
+    <t>ACME LTD - sixth expense</t>
+  </si>
+  <si>
+    <t>Acme Expenses</t>
+  </si>
+  <si>
+    <t>Bank monthly incoming transaction 01</t>
+  </si>
+  <si>
+    <t>Bank monthly incoming transaction 02</t>
+  </si>
+  <si>
+    <t>Bank monthly incoming transaction 03</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -380,6 +432,7 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -412,7 +465,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -457,6 +510,25 @@
     <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="19" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1046,352 +1118,402 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEB17BBD-6FBB-4BDC-8FD6-599D29D94644}">
-  <dimension ref="A1:I20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EB9719F-5CED-48E6-9482-9780096C1075}">
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="11"/>
+    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="B1" s="24">
-        <f>SUM(B2:B295)</f>
-        <v>9672.994999999999</v>
-      </c>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25" t="s">
-        <v>54</v>
-      </c>
-      <c r="E1" s="26"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="27">
-        <v>686.72400000000005</v>
-      </c>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28" t="s">
-        <v>60</v>
-      </c>
-      <c r="E2" s="29"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="30"/>
-      <c r="B3" s="27"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="30" t="s">
-        <v>56</v>
-      </c>
-      <c r="E3" s="29"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
-      <c r="H3" s="28"/>
-      <c r="I3" s="28"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="B4" s="29">
-        <v>72.623999999999995</v>
-      </c>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28" t="s">
-        <v>61</v>
-      </c>
-      <c r="E4" s="29"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="28"/>
-      <c r="H4" s="28"/>
-      <c r="I4" s="28"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5" s="27">
-        <v>47.259</v>
-      </c>
-      <c r="C5" s="28"/>
-      <c r="D5" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="E5" s="29"/>
-      <c r="F5" s="28"/>
-      <c r="G5" s="28"/>
-      <c r="H5" s="28"/>
-      <c r="I5" s="28"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="30"/>
-      <c r="B6" s="27"/>
-      <c r="C6" s="28"/>
-      <c r="D6" s="30" t="s">
-        <v>56</v>
-      </c>
-      <c r="E6" s="29"/>
-      <c r="F6" s="28"/>
-      <c r="G6" s="28"/>
-      <c r="H6" s="28"/>
-      <c r="I6" s="28"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="30"/>
-      <c r="B7" s="27">
-        <v>534</v>
-      </c>
-      <c r="C7" s="28"/>
-      <c r="D7" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="E7" s="29"/>
-      <c r="F7" s="28"/>
-      <c r="G7" s="28"/>
-      <c r="H7" s="28"/>
-      <c r="I7" s="28"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="30"/>
-      <c r="B8" s="27">
-        <v>70.31</v>
-      </c>
-      <c r="C8" s="28"/>
-      <c r="D8" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="E8" s="29"/>
-      <c r="F8" s="28"/>
-      <c r="G8" s="28"/>
-      <c r="H8" s="28"/>
-      <c r="I8" s="28"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="B9" s="27">
-        <v>1351.76</v>
-      </c>
-      <c r="C9" s="28"/>
-      <c r="D9" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="E9" s="29"/>
-      <c r="F9" s="28"/>
-      <c r="G9" s="28"/>
-      <c r="H9" s="28"/>
-      <c r="I9" s="28"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="30"/>
-      <c r="B10" s="27">
-        <v>168.21</v>
-      </c>
-      <c r="C10" s="28"/>
-      <c r="D10" s="30" t="s">
-        <v>66</v>
-      </c>
-      <c r="E10" s="29"/>
-      <c r="F10" s="28"/>
-      <c r="G10" s="28"/>
-      <c r="H10" s="28"/>
-      <c r="I10" s="28"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="B11" s="27">
-        <v>431.62</v>
-      </c>
-      <c r="C11" s="28"/>
-      <c r="D11" s="30" t="s">
-        <v>67</v>
-      </c>
-      <c r="E11" s="29" t="s">
-        <v>76</v>
-      </c>
-      <c r="F11" s="28" t="s">
-        <v>75</v>
-      </c>
-      <c r="G11" s="28"/>
-      <c r="H11" s="28"/>
-      <c r="I11" s="28"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="23"/>
-      <c r="B12" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="C12" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="D12" s="23" t="s">
-        <v>57</v>
-      </c>
-      <c r="E12" s="26"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="25"/>
-      <c r="H12" s="25"/>
-      <c r="I12" s="25"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="B13" s="29">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="28"/>
-      <c r="D13" s="30" t="s">
-        <v>69</v>
-      </c>
-      <c r="G13" s="28"/>
-      <c r="H13" s="28"/>
-      <c r="I13" s="28"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="B14" s="27">
-        <v>102.884</v>
-      </c>
-      <c r="C14" s="28"/>
-      <c r="D14" s="30" t="s">
-        <v>68</v>
-      </c>
-      <c r="E14" s="29"/>
-      <c r="F14" s="28"/>
-      <c r="G14" s="28"/>
-      <c r="H14" s="28"/>
-      <c r="I14" s="28"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="23"/>
-      <c r="B15" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="C15" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="D15" s="23" t="s">
-        <v>57</v>
-      </c>
-      <c r="E15" s="26"/>
-      <c r="F15" s="25"/>
-      <c r="G15" s="25"/>
-      <c r="H15" s="25"/>
-      <c r="I15" s="25"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="B16" s="27">
-        <v>1799.2239999999999</v>
-      </c>
-      <c r="C16" s="25"/>
-      <c r="D16" s="30" t="s">
-        <v>70</v>
-      </c>
-      <c r="E16" s="26"/>
-      <c r="F16" s="25"/>
-      <c r="G16" s="25"/>
-      <c r="H16" s="25"/>
-      <c r="I16" s="25"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="21" t="s">
-        <v>41</v>
-      </c>
-      <c r="B17" s="27">
-        <v>499.82400000000001</v>
-      </c>
-      <c r="C17" s="25"/>
-      <c r="D17" s="30" t="s">
-        <v>71</v>
-      </c>
-      <c r="E17" s="26"/>
-      <c r="F17" s="25"/>
-      <c r="G17" s="25"/>
-      <c r="H17" s="25"/>
-      <c r="I17" s="25"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="21" t="s">
-        <v>58</v>
-      </c>
-      <c r="B18" s="27">
-        <v>1265.2239999999999</v>
-      </c>
-      <c r="C18" s="28"/>
-      <c r="D18" s="30" t="s">
-        <v>72</v>
-      </c>
-      <c r="E18" s="29"/>
-      <c r="F18" s="28"/>
-      <c r="G18" s="28"/>
-      <c r="H18" s="28"/>
-      <c r="I18" s="28"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="21" t="s">
-        <v>59</v>
-      </c>
-      <c r="B19" s="27">
-        <v>2633.3320000000003</v>
-      </c>
-      <c r="C19" s="28"/>
-      <c r="D19" s="30" t="s">
-        <v>73</v>
-      </c>
-      <c r="E19" s="29"/>
-      <c r="F19" s="28"/>
-      <c r="G19" s="28"/>
-      <c r="H19" s="28"/>
-      <c r="I19" s="28"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="30"/>
-      <c r="B20" s="27"/>
-      <c r="C20" s="27">
-        <f>SUM(B19:B19)</f>
-        <v>2633.3320000000003</v>
-      </c>
-      <c r="D20" s="30" t="s">
-        <v>74</v>
-      </c>
-      <c r="E20" s="29"/>
-      <c r="F20" s="28"/>
-      <c r="G20" s="28"/>
-      <c r="H20" s="28"/>
-      <c r="I20" s="28"/>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>43181</v>
+      </c>
+      <c r="C2" s="11">
+        <v>12.38</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78F765B7-6603-4F53-B527-643EF2AFECBE}">
+  <dimension ref="A1:K5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" s="9" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A1" s="37" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="38" t="s">
+        <v>80</v>
+      </c>
+      <c r="D1" s="38"/>
+      <c r="E1" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="33" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="33" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" s="39" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="39" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="40">
+        <f>$J$2+K2</f>
+        <v>43617</v>
+      </c>
+      <c r="C2" s="41">
+        <v>21.762</v>
+      </c>
+      <c r="D2" s="41"/>
+      <c r="E2" s="34" t="s">
+        <v>42</v>
+      </c>
+      <c r="F2" s="39" t="s">
+        <v>92</v>
+      </c>
+      <c r="J2" s="42">
+        <v>43616</v>
+      </c>
+      <c r="K2" s="39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" s="39" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="40">
+        <f t="shared" ref="B3:B4" si="0">$J$2+K3</f>
+        <v>43618</v>
+      </c>
+      <c r="C3" s="41">
+        <v>15.600000000000001</v>
+      </c>
+      <c r="D3" s="41"/>
+      <c r="E3" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="F3" s="39" t="s">
+        <v>93</v>
+      </c>
+      <c r="J3" s="42"/>
+      <c r="K3" s="39">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" s="39" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="40">
+        <f t="shared" si="0"/>
+        <v>43619</v>
+      </c>
+      <c r="C4" s="41">
+        <v>54.974400000000003</v>
+      </c>
+      <c r="D4" s="41"/>
+      <c r="E4" s="34" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" s="39" t="s">
+        <v>94</v>
+      </c>
+      <c r="K4" s="39">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B5" s="43" t="s">
+        <v>95</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FF22F54-1C2B-49C1-90A9-21044AC295B0}">
+  <dimension ref="A1:K12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" s="9" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A1" s="16"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+    </row>
+    <row r="2" spans="1:11" s="16" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+    </row>
+    <row r="3" spans="1:11" s="16" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="20">
+        <f>$J$3+K3</f>
+        <v>43405</v>
+      </c>
+      <c r="C3" s="19">
+        <v>21.762</v>
+      </c>
+      <c r="D3" s="19"/>
+      <c r="E3" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="J3" s="22">
+        <v>43404</v>
+      </c>
+      <c r="K3" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" s="16" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="20">
+        <f t="shared" ref="B4:B10" si="0">$J$3+K4</f>
+        <v>43405</v>
+      </c>
+      <c r="C4" s="19">
+        <v>15.600000000000001</v>
+      </c>
+      <c r="D4" s="19"/>
+      <c r="E4" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="F4" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="J4" s="22"/>
+      <c r="K4" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" s="16" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="20">
+        <f t="shared" si="0"/>
+        <v>43405</v>
+      </c>
+      <c r="C5" s="19">
+        <v>54.974400000000003</v>
+      </c>
+      <c r="D5" s="19"/>
+      <c r="E5" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="I5" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="K5" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" s="16" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="20">
+        <f t="shared" si="0"/>
+        <v>43405</v>
+      </c>
+      <c r="C6" s="19">
+        <v>156</v>
+      </c>
+      <c r="D6" s="19"/>
+      <c r="E6" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="K6" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" s="16" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="20">
+        <f t="shared" si="0"/>
+        <v>43405</v>
+      </c>
+      <c r="C7" s="19">
+        <v>3.1044</v>
+      </c>
+      <c r="D7" s="19"/>
+      <c r="E7" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="F7" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="K7" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" s="16" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="20">
+        <f t="shared" si="0"/>
+        <v>43405</v>
+      </c>
+      <c r="C8" s="19">
+        <v>3.1044</v>
+      </c>
+      <c r="D8" s="19"/>
+      <c r="E8" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="K8" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" s="16" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="20">
+        <f t="shared" si="0"/>
+        <v>43405</v>
+      </c>
+      <c r="C9" s="19">
+        <v>93.82</v>
+      </c>
+      <c r="D9" s="19"/>
+      <c r="E9" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="F9" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="K9" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" s="16" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" s="20">
+        <f t="shared" si="0"/>
+        <v>43405</v>
+      </c>
+      <c r="C10" s="19">
+        <v>78</v>
+      </c>
+      <c r="D10" s="19"/>
+      <c r="E10" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="F10" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="K10" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" s="16" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A11" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" s="20">
+        <f>$J$3+K11</f>
+        <v>43405</v>
+      </c>
+      <c r="C11" s="19">
+        <v>120.83759999999999</v>
+      </c>
+      <c r="D11" s="19"/>
+      <c r="E11" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="K11" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F12" s="16"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -1554,7 +1676,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8ADEDA7-CE7F-46FB-B96B-C8F28E94F278}">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F1" sqref="F1:J11"/>
     </sheetView>
   </sheetViews>
@@ -1734,6 +1856,568 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB0AC0AE-04A7-457F-927A-C4F054F3A801}">
+  <dimension ref="A1:G11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C16" sqref="C16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="31" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" s="33" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" s="32" t="s">
+        <v>81</v>
+      </c>
+      <c r="E1" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="F1" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="G1" s="33" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="7">
+        <v>43952</v>
+      </c>
+      <c r="B2" s="14"/>
+      <c r="C2" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="14">
+        <v>5</v>
+      </c>
+      <c r="E2" s="7">
+        <v>43952</v>
+      </c>
+      <c r="F2" s="14"/>
+      <c r="G2" s="10" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="7">
+        <v>43953</v>
+      </c>
+      <c r="B3" s="14"/>
+      <c r="C3" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="14">
+        <v>10</v>
+      </c>
+      <c r="E3" s="7">
+        <v>43953</v>
+      </c>
+      <c r="F3" s="14">
+        <v>25</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="7">
+        <v>43954</v>
+      </c>
+      <c r="B4" s="14"/>
+      <c r="C4" s="34" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="14">
+        <v>15</v>
+      </c>
+      <c r="E4" s="7">
+        <v>43954</v>
+      </c>
+      <c r="F4" s="14">
+        <v>25</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="14"/>
+      <c r="F5" s="14"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="35">
+        <v>43983</v>
+      </c>
+      <c r="B6" s="14">
+        <v>20</v>
+      </c>
+      <c r="C6" t="s">
+        <v>91</v>
+      </c>
+      <c r="D6" s="14"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="14"/>
+      <c r="G6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="35">
+        <v>43984</v>
+      </c>
+      <c r="B7" s="14">
+        <v>25</v>
+      </c>
+      <c r="C7" t="s">
+        <v>91</v>
+      </c>
+      <c r="D7" s="14"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="14"/>
+      <c r="G7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="35">
+        <v>43985</v>
+      </c>
+      <c r="B8" s="14">
+        <v>30</v>
+      </c>
+      <c r="C8" t="s">
+        <v>91</v>
+      </c>
+      <c r="D8" s="14"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="14"/>
+      <c r="G8" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="35">
+        <v>43993</v>
+      </c>
+      <c r="B9" s="14">
+        <v>20</v>
+      </c>
+      <c r="C9" t="s">
+        <v>91</v>
+      </c>
+      <c r="D9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="35">
+        <v>43994</v>
+      </c>
+      <c r="B10" s="14">
+        <v>20</v>
+      </c>
+      <c r="C10" t="s">
+        <v>91</v>
+      </c>
+      <c r="D10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="35">
+        <v>43995</v>
+      </c>
+      <c r="B11" s="14">
+        <v>20</v>
+      </c>
+      <c r="C11" t="s">
+        <v>91</v>
+      </c>
+      <c r="D11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" t="s">
+        <v>90</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEB17BBD-6FBB-4BDC-8FD6-599D29D94644}">
+  <dimension ref="A1:I20"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="24">
+        <f>SUM(B2:B295)</f>
+        <v>9672.994999999999</v>
+      </c>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1" s="26"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="27">
+        <v>686.72400000000005</v>
+      </c>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2" s="29"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="30"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="E3" s="29"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
+      <c r="I3" s="28"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="29">
+        <v>72.623999999999995</v>
+      </c>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="E4" s="29"/>
+      <c r="F4" s="28"/>
+      <c r="G4" s="28"/>
+      <c r="H4" s="28"/>
+      <c r="I4" s="28"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="27">
+        <v>47.259</v>
+      </c>
+      <c r="C5" s="28"/>
+      <c r="D5" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="E5" s="29"/>
+      <c r="F5" s="28"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="28"/>
+      <c r="I5" s="28"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="30"/>
+      <c r="B6" s="27"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="E6" s="29"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="28"/>
+      <c r="I6" s="28"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="30"/>
+      <c r="B7" s="27">
+        <v>534</v>
+      </c>
+      <c r="C7" s="28"/>
+      <c r="D7" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="E7" s="29"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="28"/>
+      <c r="H7" s="28"/>
+      <c r="I7" s="28"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="30"/>
+      <c r="B8" s="27">
+        <v>70.31</v>
+      </c>
+      <c r="C8" s="28"/>
+      <c r="D8" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="E8" s="29"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="28"/>
+      <c r="I8" s="28"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="27">
+        <v>1351.76</v>
+      </c>
+      <c r="C9" s="28"/>
+      <c r="D9" s="30" t="s">
+        <v>65</v>
+      </c>
+      <c r="E9" s="29"/>
+      <c r="F9" s="28"/>
+      <c r="G9" s="28"/>
+      <c r="H9" s="28"/>
+      <c r="I9" s="28"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="30"/>
+      <c r="B10" s="27">
+        <v>168.21</v>
+      </c>
+      <c r="C10" s="28"/>
+      <c r="D10" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="E10" s="29"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="28"/>
+      <c r="H10" s="28"/>
+      <c r="I10" s="28"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" s="27">
+        <v>431.62</v>
+      </c>
+      <c r="C11" s="28"/>
+      <c r="D11" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="E11" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="F11" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="G11" s="28"/>
+      <c r="H11" s="28"/>
+      <c r="I11" s="28"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="23"/>
+      <c r="B12" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="D12" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="E12" s="26"/>
+      <c r="F12" s="25"/>
+      <c r="G12" s="25"/>
+      <c r="H12" s="25"/>
+      <c r="I12" s="25"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" s="29">
+        <v>10</v>
+      </c>
+      <c r="C13" s="28"/>
+      <c r="D13" s="30" t="s">
+        <v>69</v>
+      </c>
+      <c r="G13" s="28"/>
+      <c r="H13" s="28"/>
+      <c r="I13" s="28"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="27">
+        <v>102.884</v>
+      </c>
+      <c r="C14" s="28"/>
+      <c r="D14" s="30" t="s">
+        <v>68</v>
+      </c>
+      <c r="E14" s="29"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="28"/>
+      <c r="H14" s="28"/>
+      <c r="I14" s="28"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="23"/>
+      <c r="B15" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="C15" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="D15" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="E15" s="26"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="25"/>
+      <c r="I15" s="25"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" s="27">
+        <v>1799.2239999999999</v>
+      </c>
+      <c r="C16" s="25"/>
+      <c r="D16" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="E16" s="26"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="25"/>
+      <c r="I16" s="25"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" s="27">
+        <v>499.82400000000001</v>
+      </c>
+      <c r="C17" s="25"/>
+      <c r="D17" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="E17" s="26"/>
+      <c r="F17" s="25"/>
+      <c r="G17" s="25"/>
+      <c r="H17" s="25"/>
+      <c r="I17" s="25"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="B18" s="27">
+        <v>1265.2239999999999</v>
+      </c>
+      <c r="C18" s="28"/>
+      <c r="D18" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="E18" s="29"/>
+      <c r="F18" s="28"/>
+      <c r="G18" s="28"/>
+      <c r="H18" s="28"/>
+      <c r="I18" s="28"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="B19" s="27">
+        <v>2633.3320000000003</v>
+      </c>
+      <c r="C19" s="28"/>
+      <c r="D19" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="E19" s="29"/>
+      <c r="F19" s="28"/>
+      <c r="G19" s="28"/>
+      <c r="H19" s="28"/>
+      <c r="I19" s="28"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="30"/>
+      <c r="B20" s="27"/>
+      <c r="C20" s="27">
+        <f>SUM(B19:B19)</f>
+        <v>2633.3320000000003</v>
+      </c>
+      <c r="D20" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="E20" s="29"/>
+      <c r="F20" s="28"/>
+      <c r="G20" s="28"/>
+      <c r="H20" s="28"/>
+      <c r="I20" s="28"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6113D0FC-182D-42CE-86C5-3C69DBF97D2B}">
   <dimension ref="A1:E12"/>
   <sheetViews>
@@ -1891,7 +2575,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{200A4C87-1C2C-4B37-A6E6-AE9D20363943}">
   <dimension ref="A1:E3"/>
   <sheetViews>
@@ -1954,7 +2638,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EA57B23-4855-4496-A701-3354AE195B0D}">
   <dimension ref="A1:E23"/>
   <sheetViews>
@@ -2200,289 +2884,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EB9719F-5CED-48E6-9482-9780096C1075}">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="11"/>
-    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>43181</v>
-      </c>
-      <c r="C2" s="11">
-        <v>12.38</v>
-      </c>
-      <c r="D2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FF22F54-1C2B-49C1-90A9-21044AC295B0}">
-  <dimension ref="A1:K12"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="35.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" s="9" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A1" s="16"/>
-      <c r="B1" s="17"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-    </row>
-    <row r="2" spans="1:11" s="16" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-    </row>
-    <row r="3" spans="1:11" s="16" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="B3" s="20">
-        <f>$J$3+K3</f>
-        <v>43405</v>
-      </c>
-      <c r="C3" s="19">
-        <v>21.762</v>
-      </c>
-      <c r="D3" s="19"/>
-      <c r="E3" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="F3" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="J3" s="22">
-        <v>43404</v>
-      </c>
-      <c r="K3" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" s="16" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="B4" s="20">
-        <f t="shared" ref="B4:B10" si="0">$J$3+K4</f>
-        <v>43405</v>
-      </c>
-      <c r="C4" s="19">
-        <v>15.600000000000001</v>
-      </c>
-      <c r="D4" s="19"/>
-      <c r="E4" s="21" t="s">
-        <v>44</v>
-      </c>
-      <c r="F4" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="J4" s="22"/>
-      <c r="K4" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" s="16" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5" s="20">
-        <f t="shared" si="0"/>
-        <v>43405</v>
-      </c>
-      <c r="C5" s="19">
-        <v>54.974400000000003</v>
-      </c>
-      <c r="D5" s="19"/>
-      <c r="E5" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="F5" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="I5" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="K5" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" s="16" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="B6" s="20">
-        <f t="shared" si="0"/>
-        <v>43405</v>
-      </c>
-      <c r="C6" s="19">
-        <v>156</v>
-      </c>
-      <c r="D6" s="19"/>
-      <c r="E6" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="F6" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="K6" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" s="16" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="B7" s="20">
-        <f t="shared" si="0"/>
-        <v>43405</v>
-      </c>
-      <c r="C7" s="19">
-        <v>3.1044</v>
-      </c>
-      <c r="D7" s="19"/>
-      <c r="E7" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="F7" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="K7" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" s="16" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="B8" s="20">
-        <f t="shared" si="0"/>
-        <v>43405</v>
-      </c>
-      <c r="C8" s="19">
-        <v>3.1044</v>
-      </c>
-      <c r="D8" s="19"/>
-      <c r="E8" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="F8" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="K8" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" s="16" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="B9" s="20">
-        <f t="shared" si="0"/>
-        <v>43405</v>
-      </c>
-      <c r="C9" s="19">
-        <v>93.82</v>
-      </c>
-      <c r="D9" s="19"/>
-      <c r="E9" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="F9" s="16" t="s">
-        <v>78</v>
-      </c>
-      <c r="K9" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" s="16" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="B10" s="20">
-        <f t="shared" si="0"/>
-        <v>43405</v>
-      </c>
-      <c r="C10" s="19">
-        <v>78</v>
-      </c>
-      <c r="D10" s="19"/>
-      <c r="E10" s="21" t="s">
-        <v>44</v>
-      </c>
-      <c r="F10" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="K10" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" s="16" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A11" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="B11" s="20">
-        <f>$J$3+K11</f>
-        <v>43405</v>
-      </c>
-      <c r="C11" s="19">
-        <v>120.83759999999999</v>
-      </c>
-      <c r="D11" s="19"/>
-      <c r="E11" s="21" t="s">
-        <v>44</v>
-      </c>
-      <c r="F11" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="K11" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F12" s="16"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Moved LastTransactionMarker from BankRecord to ActualBankRecord and got it working.
</commit_message>
<xml_diff>
--- a/spreadsheet-samples/Test-Spreadsheet.xlsx
+++ b/spreadsheet-samples/Test-Spreadsheet.xlsx
@@ -8,26 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\development\Reconciliate\spreadsheet-samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C9859E7-665E-41DD-ADC6-194F8C9B4EBC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FE7FFE2-8258-43FC-B2FA-9054009CE87C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="75" yWindow="225" windowWidth="22905" windowHeight="12285" firstSheet="5" activeTab="10" xr2:uid="{E73E5FC3-A692-4EF9-93A1-0012994854D9}"/>
+    <workbookView xWindow="24525" yWindow="1065" windowWidth="18525" windowHeight="12285" xr2:uid="{E73E5FC3-A692-4EF9-93A1-0012994854D9}"/>
   </bookViews>
   <sheets>
     <sheet name="Bank" sheetId="7" r:id="rId1"/>
-    <sheet name="ActualBank" sheetId="2" r:id="rId2"/>
-    <sheet name="CredCard1" sheetId="6" r:id="rId3"/>
-    <sheet name="CredCard" sheetId="3" r:id="rId4"/>
-    <sheet name="Expected In" sheetId="11" r:id="rId5"/>
-    <sheet name="Expected Out" sheetId="10" r:id="rId6"/>
-    <sheet name="ForDeletingUnreconciled" sheetId="9" r:id="rId7"/>
-    <sheet name="BadDivider" sheetId="8" r:id="rId8"/>
-    <sheet name="TestRecord" sheetId="1" r:id="rId9"/>
-    <sheet name="CredCard2" sheetId="5" r:id="rId10"/>
-    <sheet name="Budget In" sheetId="12" r:id="rId11"/>
-    <sheet name="Budget Out" sheetId="4" r:id="rId12"/>
+    <sheet name="CredCard1" sheetId="6" r:id="rId2"/>
+    <sheet name="CredCard" sheetId="3" r:id="rId3"/>
+    <sheet name="Expected In" sheetId="11" r:id="rId4"/>
+    <sheet name="Expected Out" sheetId="10" r:id="rId5"/>
+    <sheet name="ForDeletingUnreconciled" sheetId="9" r:id="rId6"/>
+    <sheet name="BadDivider" sheetId="8" r:id="rId7"/>
+    <sheet name="TestRecord" sheetId="1" r:id="rId8"/>
+    <sheet name="CredCard2" sheetId="5" r:id="rId9"/>
+    <sheet name="Budget In" sheetId="12" r:id="rId10"/>
+    <sheet name="Budget Out" sheetId="4" r:id="rId11"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId13"/>
+    <externalReference r:id="rId12"/>
   </externalReferences>
   <definedNames>
     <definedName name="Actual_Gross">#REF!</definedName>
@@ -86,7 +85,7 @@
     <definedName name="VATRate">#REF!</definedName>
     <definedName name="VATRateToHMRC">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -104,7 +103,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="88">
   <si>
     <t>Col1</t>
   </si>
@@ -127,12 +126,6 @@
     <t>description</t>
   </si>
   <si>
-    <t>notes</t>
-  </si>
-  <si>
-    <t>info</t>
-  </si>
-  <si>
     <t>Date</t>
   </si>
   <si>
@@ -160,9 +153,6 @@
     <t>Vendor Id</t>
   </si>
   <si>
-    <t>Balance</t>
-  </si>
-  <si>
     <t>Thing</t>
   </si>
   <si>
@@ -172,33 +162,15 @@
     <t>description1</t>
   </si>
   <si>
-    <t>notes1</t>
-  </si>
-  <si>
-    <t>info1</t>
-  </si>
-  <si>
     <t>description2</t>
   </si>
   <si>
-    <t>notes2</t>
-  </si>
-  <si>
-    <t>info2</t>
-  </si>
-  <si>
     <t>description3</t>
   </si>
   <si>
     <t>description4</t>
   </si>
   <si>
-    <t>notes4</t>
-  </si>
-  <si>
-    <t>info4</t>
-  </si>
-  <si>
     <t>pintipoplication</t>
   </si>
   <si>
@@ -392,6 +364,9 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>!! Last online transaction!!</t>
   </si>
 </sst>
 </file>
@@ -465,7 +440,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -530,6 +505,8 @@
     <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -944,10 +921,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B106CA6-6EF5-459F-BBFA-85FA2D21E2D2}">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:J7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -957,29 +934,31 @@
     <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.28515625" style="13" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15" style="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.7109375" style="44" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="F1" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="E1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F1" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="G1" s="11" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="7">
         <v>43249</v>
       </c>
@@ -988,7 +967,7 @@
       </c>
       <c r="C2" s="8"/>
       <c r="D2" s="9" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="E2" s="10" t="s">
         <v>6</v>
@@ -999,21 +978,29 @@
       <c r="G2" s="8">
         <v>4567.8900000000003</v>
       </c>
-      <c r="H2" s="9" t="s">
-        <v>7</v>
-      </c>
+      <c r="H2" s="9"/>
       <c r="I2" s="9"/>
-      <c r="J2" s="9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J2" s="9"/>
+      <c r="L2" s="7">
+        <v>43250</v>
+      </c>
+      <c r="M2" s="45">
+        <v>4567.8900000000003</v>
+      </c>
+      <c r="N2" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="O2" s="10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B3" s="14" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G3" s="14"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>43280</v>
       </c>
@@ -1022,10 +1009,10 @@
       </c>
       <c r="C4" s="15"/>
       <c r="D4" s="9" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F4" s="12">
         <v>12345</v>
@@ -1033,15 +1020,23 @@
       <c r="G4" s="15">
         <v>4567.8900000000003</v>
       </c>
-      <c r="H4" s="9" t="s">
-        <v>22</v>
-      </c>
+      <c r="H4" s="9"/>
       <c r="I4" s="9"/>
-      <c r="J4" s="9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J4" s="9"/>
+      <c r="L4" s="7">
+        <v>43250</v>
+      </c>
+      <c r="M4" s="45">
+        <v>4567.8900000000003</v>
+      </c>
+      <c r="N4" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="O4" s="10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>43281</v>
       </c>
@@ -1049,10 +1044,10 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="F5" s="13">
         <v>22345</v>
@@ -1060,14 +1055,21 @@
       <c r="G5" s="14">
         <v>5567.89</v>
       </c>
-      <c r="H5" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="J5" s="9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J5" s="9"/>
+      <c r="L5" s="7">
+        <v>43250</v>
+      </c>
+      <c r="M5" s="45">
+        <v>4567.8900000000003</v>
+      </c>
+      <c r="N5" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="O5" s="10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>43282</v>
       </c>
@@ -1075,17 +1077,17 @@
         <v>5.15</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="F6" s="12"/>
       <c r="G6" s="15"/>
       <c r="H6" s="9"/>
       <c r="J6" s="9"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>43283</v>
       </c>
@@ -1093,10 +1095,10 @@
         <v>5.2</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="F7" s="13">
         <v>42345</v>
@@ -1104,11 +1106,21 @@
       <c r="G7" s="14">
         <v>7567.89</v>
       </c>
-      <c r="H7" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="J7" s="9" t="s">
-        <v>30</v>
+      <c r="H7" t="s">
+        <v>87</v>
+      </c>
+      <c r="J7" s="9"/>
+      <c r="L7" s="7">
+        <v>43250</v>
+      </c>
+      <c r="M7" s="45">
+        <v>4567.8900000000003</v>
+      </c>
+      <c r="N7" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="O7" s="10" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -1118,53 +1130,10 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EB9719F-5CED-48E6-9482-9780096C1075}">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="11"/>
-    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>43181</v>
-      </c>
-      <c r="C2" s="11">
-        <v>12.38</v>
-      </c>
-      <c r="D2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78F765B7-6603-4F53-B527-643EF2AFECBE}">
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
@@ -1176,28 +1145,28 @@
   <sheetData>
     <row r="1" spans="1:11" s="9" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="37" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="B1" s="33" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C1" s="38" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="D1" s="38"/>
       <c r="E1" s="33" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F1" s="33" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G1" s="33" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:11" s="39" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="39" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="B2" s="40">
         <f>$J$2+K2</f>
@@ -1208,10 +1177,10 @@
       </c>
       <c r="D2" s="41"/>
       <c r="E2" s="34" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="F2" s="39" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="J2" s="42">
         <v>43616</v>
@@ -1222,7 +1191,7 @@
     </row>
     <row r="3" spans="1:11" s="39" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="39" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="B3" s="40">
         <f t="shared" ref="B3:B4" si="0">$J$2+K3</f>
@@ -1233,10 +1202,10 @@
       </c>
       <c r="D3" s="41"/>
       <c r="E3" s="34" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="F3" s="39" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="J3" s="42"/>
       <c r="K3" s="39">
@@ -1245,7 +1214,7 @@
     </row>
     <row r="4" spans="1:11" s="39" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="39" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="B4" s="40">
         <f t="shared" si="0"/>
@@ -1256,10 +1225,10 @@
       </c>
       <c r="D4" s="41"/>
       <c r="E4" s="34" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="F4" s="39" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="K4" s="39">
         <v>3</v>
@@ -1267,7 +1236,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B5" s="43" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -1275,7 +1244,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FF22F54-1C2B-49C1-90A9-21044AC295B0}">
   <dimension ref="A1:K12"/>
   <sheetViews>
@@ -1299,14 +1268,14 @@
     </row>
     <row r="2" spans="1:11" s="16" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="18" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="C2" s="19"/>
       <c r="D2" s="19"/>
     </row>
     <row r="3" spans="1:11" s="16" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="16" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="B3" s="20">
         <f>$J$3+K3</f>
@@ -1317,10 +1286,10 @@
       </c>
       <c r="D3" s="19"/>
       <c r="E3" s="21" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="F3" s="16" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="J3" s="22">
         <v>43404</v>
@@ -1331,7 +1300,7 @@
     </row>
     <row r="4" spans="1:11" s="16" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="B4" s="20">
         <f t="shared" ref="B4:B10" si="0">$J$3+K4</f>
@@ -1342,10 +1311,10 @@
       </c>
       <c r="D4" s="19"/>
       <c r="E4" s="21" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="F4" s="16" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="J4" s="22"/>
       <c r="K4" s="16">
@@ -1354,7 +1323,7 @@
     </row>
     <row r="5" spans="1:11" s="16" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="16" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="B5" s="20">
         <f t="shared" si="0"/>
@@ -1365,10 +1334,10 @@
       </c>
       <c r="D5" s="19"/>
       <c r="E5" s="21" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="F5" s="16" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="I5" s="16" t="s">
         <v>4</v>
@@ -1379,7 +1348,7 @@
     </row>
     <row r="6" spans="1:11" s="16" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="16" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="B6" s="20">
         <f t="shared" si="0"/>
@@ -1390,10 +1359,10 @@
       </c>
       <c r="D6" s="19"/>
       <c r="E6" s="21" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="F6" s="16" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="K6" s="16">
         <v>1</v>
@@ -1401,7 +1370,7 @@
     </row>
     <row r="7" spans="1:11" s="16" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="16" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="B7" s="20">
         <f t="shared" si="0"/>
@@ -1412,10 +1381,10 @@
       </c>
       <c r="D7" s="19"/>
       <c r="E7" s="21" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="F7" s="16" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="K7" s="16">
         <v>1</v>
@@ -1423,7 +1392,7 @@
     </row>
     <row r="8" spans="1:11" s="16" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="16" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="B8" s="20">
         <f t="shared" si="0"/>
@@ -1434,10 +1403,10 @@
       </c>
       <c r="D8" s="19"/>
       <c r="E8" s="21" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="F8" s="16" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="K8" s="16">
         <v>1</v>
@@ -1445,7 +1414,7 @@
     </row>
     <row r="9" spans="1:11" s="16" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="16" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="B9" s="20">
         <f t="shared" si="0"/>
@@ -1456,10 +1425,10 @@
       </c>
       <c r="D9" s="19"/>
       <c r="E9" s="21" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="F9" s="16" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="K9" s="16">
         <v>1</v>
@@ -1467,7 +1436,7 @@
     </row>
     <row r="10" spans="1:11" s="16" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="16" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="B10" s="20">
         <f t="shared" si="0"/>
@@ -1478,10 +1447,10 @@
       </c>
       <c r="D10" s="19"/>
       <c r="E10" s="21" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="F10" s="16" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="K10" s="16">
         <v>1</v>
@@ -1489,7 +1458,7 @@
     </row>
     <row r="11" spans="1:11" s="16" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="16" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="B11" s="20">
         <f>$J$3+K11</f>
@@ -1500,10 +1469,10 @@
       </c>
       <c r="D11" s="19"/>
       <c r="E11" s="21" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="F11" s="16" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="K11" s="16">
         <v>1</v>
@@ -1518,63 +1487,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3917BA43-EB48-4061-80BC-E36EE193A65C}">
-  <dimension ref="A1:F2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15" style="11" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="7">
-        <v>43250</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="8">
-        <v>4567.8900000000003</v>
-      </c>
-      <c r="E2" s="8">
-        <v>7898.88</v>
-      </c>
-      <c r="F2" s="9"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D874970E-DFC7-41AF-9C75-179A4BAE8469}">
   <dimension ref="A1:D6"/>
   <sheetViews>
@@ -1592,16 +1504,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="C1" t="s">
-        <v>11</v>
-      </c>
       <c r="D1" s="14" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1620,7 +1532,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3" s="14" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D3"/>
     </row>
@@ -1632,7 +1544,7 @@
         <v>66589</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D4" s="15">
         <v>37956.9</v>
@@ -1646,7 +1558,7 @@
         <v>66590</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D5" s="15">
         <v>37957.9</v>
@@ -1660,7 +1572,7 @@
         <v>66591</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="D6" s="15">
         <v>37958.9</v>
@@ -1672,7 +1584,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8ADEDA7-CE7F-46FB-B96B-C8F28E94F278}">
   <dimension ref="A1:J11"/>
   <sheetViews>
@@ -1697,7 +1609,7 @@
         <v>4.5</v>
       </c>
       <c r="D1" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="E1" s="6">
         <v>4567.8900000000003</v>
@@ -1707,7 +1619,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B2" s="14" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E2" s="14"/>
     </row>
@@ -1719,7 +1631,7 @@
         <v>4.5</v>
       </c>
       <c r="D3" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="E3" s="14">
         <v>4567.8900000000003</v>
@@ -1738,7 +1650,7 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="D4" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="E4" s="14">
         <v>5567.89</v>
@@ -1751,7 +1663,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B5" s="14" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E5" s="14"/>
     </row>
@@ -1763,7 +1675,7 @@
         <v>4.7</v>
       </c>
       <c r="D6" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="E6" s="14">
         <v>6567.89</v>
@@ -1781,7 +1693,7 @@
         <v>4.8</v>
       </c>
       <c r="D7" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="E7" s="14">
         <v>7567.89</v>
@@ -1799,7 +1711,7 @@
         <v>4.9000000000000004</v>
       </c>
       <c r="D8" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="E8" s="14"/>
       <c r="F8" s="13"/>
@@ -1809,7 +1721,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="14" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E9" s="14"/>
     </row>
@@ -1821,7 +1733,7 @@
         <v>5</v>
       </c>
       <c r="D10" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="E10" s="14">
         <v>9567.89</v>
@@ -1839,7 +1751,7 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="D11" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="E11" s="14">
         <v>10567.89</v>
@@ -1855,7 +1767,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB0AC0AE-04A7-457F-927A-C4F054F3A801}">
   <dimension ref="A1:G11"/>
   <sheetViews>
@@ -1874,25 +1786,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="E1" s="31" t="s">
+        <v>73</v>
+      </c>
+      <c r="F1" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="G1" s="33" t="s">
         <v>9</v>
-      </c>
-      <c r="B1" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="C1" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="D1" s="32" t="s">
-        <v>81</v>
-      </c>
-      <c r="E1" s="31" t="s">
-        <v>82</v>
-      </c>
-      <c r="F1" s="32" t="s">
-        <v>83</v>
-      </c>
-      <c r="G1" s="33" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1901,7 +1813,7 @@
       </c>
       <c r="B2" s="14"/>
       <c r="C2" s="34" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="D2" s="14">
         <v>5</v>
@@ -1911,7 +1823,7 @@
       </c>
       <c r="F2" s="14"/>
       <c r="G2" s="10" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1920,7 +1832,7 @@
       </c>
       <c r="B3" s="14"/>
       <c r="C3" s="34" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="D3" s="14">
         <v>10</v>
@@ -1932,7 +1844,7 @@
         <v>25</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1941,7 +1853,7 @@
       </c>
       <c r="B4" s="14"/>
       <c r="C4" s="34" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="D4" s="14">
         <v>15</v>
@@ -1953,12 +1865,12 @@
         <v>25</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" s="15" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D5" s="14"/>
       <c r="F5" s="14"/>
@@ -1971,13 +1883,13 @@
         <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="D6" s="14"/>
       <c r="E6" s="36"/>
       <c r="F6" s="14"/>
       <c r="G6" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1988,13 +1900,13 @@
         <v>25</v>
       </c>
       <c r="C7" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="D7" s="14"/>
       <c r="E7" s="36"/>
       <c r="F7" s="14"/>
       <c r="G7" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -2005,13 +1917,13 @@
         <v>30</v>
       </c>
       <c r="C8" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="D8" s="14"/>
       <c r="E8" s="36"/>
       <c r="F8" s="14"/>
       <c r="G8" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -2022,12 +1934,12 @@
         <v>20</v>
       </c>
       <c r="C9" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="D9" s="14"/>
       <c r="F9" s="14"/>
       <c r="G9" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -2038,12 +1950,12 @@
         <v>20</v>
       </c>
       <c r="C10" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="D10" s="14"/>
       <c r="F10" s="14"/>
       <c r="G10" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -2054,12 +1966,12 @@
         <v>20</v>
       </c>
       <c r="C11" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="D11" s="14"/>
       <c r="F11" s="14"/>
       <c r="G11" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -2067,7 +1979,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEB17BBD-6FBB-4BDC-8FD6-599D29D94644}">
   <dimension ref="A1:I20"/>
   <sheetViews>
@@ -2085,7 +1997,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="23" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="B1" s="24">
         <f>SUM(B2:B295)</f>
@@ -2093,7 +2005,7 @@
       </c>
       <c r="C1" s="25"/>
       <c r="D1" s="25" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="E1" s="26"/>
       <c r="F1" s="25"/>
@@ -2103,14 +2015,14 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="B2" s="27">
         <v>686.72400000000005</v>
       </c>
       <c r="C2" s="28"/>
       <c r="D2" s="28" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="E2" s="29"/>
       <c r="F2" s="28"/>
@@ -2123,7 +2035,7 @@
       <c r="B3" s="27"/>
       <c r="C3" s="28"/>
       <c r="D3" s="30" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="E3" s="29"/>
       <c r="F3" s="28"/>
@@ -2133,14 +2045,14 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="B4" s="29">
         <v>72.623999999999995</v>
       </c>
       <c r="C4" s="28"/>
       <c r="D4" s="28" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="E4" s="29"/>
       <c r="F4" s="28"/>
@@ -2150,14 +2062,14 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="B5" s="27">
         <v>47.259</v>
       </c>
       <c r="C5" s="28"/>
       <c r="D5" s="30" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="E5" s="29"/>
       <c r="F5" s="28"/>
@@ -2170,7 +2082,7 @@
       <c r="B6" s="27"/>
       <c r="C6" s="28"/>
       <c r="D6" s="30" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="E6" s="29"/>
       <c r="F6" s="28"/>
@@ -2185,7 +2097,7 @@
       </c>
       <c r="C7" s="28"/>
       <c r="D7" s="30" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="E7" s="29"/>
       <c r="F7" s="28"/>
@@ -2200,7 +2112,7 @@
       </c>
       <c r="C8" s="28"/>
       <c r="D8" s="30" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="E8" s="29"/>
       <c r="F8" s="28"/>
@@ -2210,14 +2122,14 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="21" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="B9" s="27">
         <v>1351.76</v>
       </c>
       <c r="C9" s="28"/>
       <c r="D9" s="30" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="E9" s="29"/>
       <c r="F9" s="28"/>
@@ -2232,7 +2144,7 @@
       </c>
       <c r="C10" s="28"/>
       <c r="D10" s="30" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="E10" s="29"/>
       <c r="F10" s="28"/>
@@ -2242,20 +2154,20 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="21" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="B11" s="27">
         <v>431.62</v>
       </c>
       <c r="C11" s="28"/>
       <c r="D11" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="E11" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="E11" s="29" t="s">
-        <v>76</v>
-      </c>
       <c r="F11" s="28" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="G11" s="28"/>
       <c r="H11" s="28"/>
@@ -2264,13 +2176,13 @@
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="23"/>
       <c r="B12" s="25" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="C12" s="25" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="D12" s="23" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E12" s="26"/>
       <c r="F12" s="25"/>
@@ -2280,14 +2192,14 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="21" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="B13" s="29">
         <v>10</v>
       </c>
       <c r="C13" s="28"/>
       <c r="D13" s="30" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="G13" s="28"/>
       <c r="H13" s="28"/>
@@ -2295,14 +2207,14 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="21" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="B14" s="27">
         <v>102.884</v>
       </c>
       <c r="C14" s="28"/>
       <c r="D14" s="30" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="E14" s="29"/>
       <c r="F14" s="28"/>
@@ -2313,13 +2225,13 @@
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="23"/>
       <c r="B15" s="25" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="C15" s="25" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="D15" s="23" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E15" s="26"/>
       <c r="F15" s="25"/>
@@ -2329,14 +2241,14 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="21" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="B16" s="27">
         <v>1799.2239999999999</v>
       </c>
       <c r="C16" s="25"/>
       <c r="D16" s="30" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="E16" s="26"/>
       <c r="F16" s="25"/>
@@ -2346,14 +2258,14 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="21" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="B17" s="27">
         <v>499.82400000000001</v>
       </c>
       <c r="C17" s="25"/>
       <c r="D17" s="30" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="E17" s="26"/>
       <c r="F17" s="25"/>
@@ -2363,14 +2275,14 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="21" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="B18" s="27">
         <v>1265.2239999999999</v>
       </c>
       <c r="C18" s="28"/>
       <c r="D18" s="30" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="E18" s="29"/>
       <c r="F18" s="28"/>
@@ -2380,14 +2292,14 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="21" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="B19" s="27">
         <v>2633.3320000000003</v>
       </c>
       <c r="C19" s="28"/>
       <c r="D19" s="30" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="E19" s="29"/>
       <c r="F19" s="28"/>
@@ -2403,7 +2315,7 @@
         <v>2633.3320000000003</v>
       </c>
       <c r="D20" s="30" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="E20" s="29"/>
       <c r="F20" s="28"/>
@@ -2417,7 +2329,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6113D0FC-182D-42CE-86C5-3C69DBF97D2B}">
   <dimension ref="A1:E12"/>
   <sheetViews>
@@ -2440,7 +2352,7 @@
         <v>4.5</v>
       </c>
       <c r="D1" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="E1" s="14">
         <v>4567.8900000000003</v>
@@ -2449,7 +2361,7 @@
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="14" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E2" s="14"/>
     </row>
@@ -2461,7 +2373,7 @@
         <v>4.5</v>
       </c>
       <c r="D3" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="E3" s="14">
         <v>4567.8900000000003</v>
@@ -2475,7 +2387,7 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="D4" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="E4" s="14">
         <v>5567.89</v>
@@ -2484,7 +2396,7 @@
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="14" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E5" s="14"/>
     </row>
@@ -2496,7 +2408,7 @@
         <v>4.7</v>
       </c>
       <c r="D6" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="E6" s="14">
         <v>6567.89</v>
@@ -2510,7 +2422,7 @@
         <v>4.8</v>
       </c>
       <c r="D7" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="E7" s="14">
         <v>7567.89</v>
@@ -2524,7 +2436,7 @@
         <v>4.9000000000000004</v>
       </c>
       <c r="D8" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="E8" s="14">
         <v>8567.89</v>
@@ -2533,7 +2445,7 @@
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="14" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E9" s="14"/>
     </row>
@@ -2545,7 +2457,7 @@
         <v>5</v>
       </c>
       <c r="D10" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="E10" s="14">
         <v>9567.89</v>
@@ -2559,7 +2471,7 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="D11" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="E11" s="14">
         <v>10567.89</v>
@@ -2567,7 +2479,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -2575,7 +2487,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{200A4C87-1C2C-4B37-A6E6-AE9D20363943}">
   <dimension ref="A1:E3"/>
   <sheetViews>
@@ -2599,7 +2511,7 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="D1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E1" s="14">
         <v>10567.89</v>
@@ -2613,7 +2525,7 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E2" s="14">
         <v>10567.89</v>
@@ -2627,7 +2539,7 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="C3" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="E3" s="14">
         <v>10567.89</v>
@@ -2638,7 +2550,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EA57B23-4855-4496-A701-3354AE195B0D}">
   <dimension ref="A1:E23"/>
   <sheetViews>
@@ -2794,7 +2706,7 @@
         <v>1242</v>
       </c>
       <c r="E10" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -2878,6 +2790,49 @@
     <row r="23" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D23">
         <v>1255</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EB9719F-5CED-48E6-9482-9780096C1075}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="11"/>
+    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>43181</v>
+      </c>
+      <c r="C2" s="11">
+        <v>12.38</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>